<commit_message>
excel now converted into a list of blocks and corresponding dictionaries for stations, switches etc
</commit_message>
<xml_diff>
--- a/src/Track/TrackModel/GreenLine_Layout.xlsx
+++ b/src/Track/TrackModel/GreenLine_Layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cjame\Documents\ECE1140ChooChoo\src\Track\TrackModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D00A9D0-B9E0-418B-BA75-2DC154E7E3A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA70F400-791D-4721-AFC1-AF13C9A34895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2700" windowWidth="29040" windowHeight="15840" xr2:uid="{85290365-C1DC-46B7-8A8F-B8FE040B733E}"/>
   </bookViews>
@@ -641,7 +641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{521756E0-942E-44A0-8B9B-C1C5C2AAFFBA}">
   <dimension ref="A1:T151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="74" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
       <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
@@ -778,7 +778,7 @@
         <v>0</v>
       </c>
       <c r="S2">
-        <f>_xlfn.FLOOR.MATH(F2*0.621371)</f>
+        <f t="shared" ref="S2:S33" si="0">_xlfn.FLOOR.MATH(F2*0.621371)</f>
         <v>27</v>
       </c>
       <c r="T2">
@@ -836,11 +836,11 @@
         <v>0</v>
       </c>
       <c r="S3">
-        <f>_xlfn.FLOOR.MATH(F3*0.621371)</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="T3">
-        <f t="shared" ref="T3:T66" si="0">D3 * 1.09361</f>
+        <f t="shared" ref="T3:T66" si="1">D3 * 1.09361</f>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -890,11 +890,11 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <f>_xlfn.FLOOR.MATH(F4*0.621371)</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="T4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -944,11 +944,11 @@
         <v>0</v>
       </c>
       <c r="S5">
-        <f>_xlfn.FLOOR.MATH(F5*0.621371)</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="T5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -998,11 +998,11 @@
         <v>0</v>
       </c>
       <c r="S6">
-        <f>_xlfn.FLOOR.MATH(F6*0.621371)</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="T6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -1052,11 +1052,11 @@
         <v>0</v>
       </c>
       <c r="S7">
-        <f>_xlfn.FLOOR.MATH(F7*0.621371)</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="T7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -1106,11 +1106,11 @@
         <v>0</v>
       </c>
       <c r="S8">
-        <f>_xlfn.FLOOR.MATH(F8*0.621371)</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="T8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -1160,11 +1160,11 @@
         <v>0</v>
       </c>
       <c r="S9">
-        <f>_xlfn.FLOOR.MATH(F9*0.621371)</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="T9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -1218,11 +1218,11 @@
         <v>0</v>
       </c>
       <c r="S10">
-        <f>_xlfn.FLOOR.MATH(F10*0.621371)</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="T10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -1272,11 +1272,11 @@
         <v>0</v>
       </c>
       <c r="S11">
-        <f>_xlfn.FLOOR.MATH(F11*0.621371)</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="T11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -1326,11 +1326,11 @@
         <v>0</v>
       </c>
       <c r="S12">
-        <f>_xlfn.FLOOR.MATH(F12*0.621371)</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="T12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -1384,11 +1384,11 @@
         <v>0</v>
       </c>
       <c r="S13">
-        <f>_xlfn.FLOOR.MATH(F13*0.621371)</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="T13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -1438,11 +1438,11 @@
         <v>0</v>
       </c>
       <c r="S14">
-        <f>_xlfn.FLOOR.MATH(F14*0.621371)</f>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="T14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>164.04149999999998</v>
       </c>
     </row>
@@ -1492,11 +1492,11 @@
         <v>0</v>
       </c>
       <c r="S15">
-        <f>_xlfn.FLOOR.MATH(F15*0.621371)</f>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="T15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>164.04149999999998</v>
       </c>
     </row>
@@ -1546,11 +1546,11 @@
         <v>0</v>
       </c>
       <c r="S16">
-        <f>_xlfn.FLOOR.MATH(F16*0.621371)</f>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="T16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>164.04149999999998</v>
       </c>
     </row>
@@ -1604,11 +1604,11 @@
         <v>0</v>
       </c>
       <c r="S17">
-        <f>_xlfn.FLOOR.MATH(F17*0.621371)</f>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="T17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>164.04149999999998</v>
       </c>
     </row>
@@ -1658,11 +1658,11 @@
         <v>0</v>
       </c>
       <c r="S18">
-        <f>_xlfn.FLOOR.MATH(F18*0.621371)</f>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="T18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>164.04149999999998</v>
       </c>
     </row>
@@ -1712,11 +1712,11 @@
         <v>0</v>
       </c>
       <c r="S19">
-        <f>_xlfn.FLOOR.MATH(F19*0.621371)</f>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="T19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>164.04149999999998</v>
       </c>
     </row>
@@ -1766,11 +1766,11 @@
         <v>0</v>
       </c>
       <c r="S20">
-        <f>_xlfn.FLOOR.MATH(F20*0.621371)</f>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="T20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>164.04149999999998</v>
       </c>
     </row>
@@ -1820,11 +1820,11 @@
         <v>0</v>
       </c>
       <c r="S21">
-        <f>_xlfn.FLOOR.MATH(F21*0.621371)</f>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="T21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>164.04149999999998</v>
       </c>
     </row>
@@ -1874,11 +1874,11 @@
         <v>0</v>
       </c>
       <c r="S22">
-        <f>_xlfn.FLOOR.MATH(F22*0.621371)</f>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="T22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>328.08299999999997</v>
       </c>
     </row>
@@ -1932,11 +1932,11 @@
         <v>0</v>
       </c>
       <c r="S23">
-        <f>_xlfn.FLOOR.MATH(F23*0.621371)</f>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="T23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>328.08299999999997</v>
       </c>
     </row>
@@ -1986,11 +1986,11 @@
         <v>0</v>
       </c>
       <c r="S24">
-        <f>_xlfn.FLOOR.MATH(F24*0.621371)</f>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="T24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>328.08299999999997</v>
       </c>
     </row>
@@ -2040,11 +2040,11 @@
         <v>0</v>
       </c>
       <c r="S25">
-        <f>_xlfn.FLOOR.MATH(F25*0.621371)</f>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="T25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>328.08299999999997</v>
       </c>
     </row>
@@ -2094,11 +2094,11 @@
         <v>0</v>
       </c>
       <c r="S26">
-        <f>_xlfn.FLOOR.MATH(F26*0.621371)</f>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="T26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>218.72199999999998</v>
       </c>
     </row>
@@ -2148,11 +2148,11 @@
         <v>0</v>
       </c>
       <c r="S27">
-        <f>_xlfn.FLOOR.MATH(F27*0.621371)</f>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="T27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -2202,11 +2202,11 @@
         <v>0</v>
       </c>
       <c r="S28">
-        <f>_xlfn.FLOOR.MATH(F28*0.621371)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="T28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -2258,11 +2258,11 @@
         <v>0</v>
       </c>
       <c r="S29">
-        <f>_xlfn.FLOOR.MATH(F29*0.621371)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="T29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -2314,11 +2314,11 @@
         <v>0</v>
       </c>
       <c r="S30">
-        <f>_xlfn.FLOOR.MATH(F30*0.621371)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="T30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -2368,11 +2368,11 @@
         <v>0</v>
       </c>
       <c r="S31">
-        <f>_xlfn.FLOOR.MATH(F31*0.621371)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="T31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -2426,11 +2426,11 @@
         <v>0</v>
       </c>
       <c r="S32">
-        <f>_xlfn.FLOOR.MATH(F32*0.621371)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="T32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -2480,11 +2480,11 @@
         <v>0</v>
       </c>
       <c r="S33">
-        <f>_xlfn.FLOOR.MATH(F33*0.621371)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="T33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -2534,11 +2534,11 @@
         <v>0</v>
       </c>
       <c r="S34">
-        <f>_xlfn.FLOOR.MATH(F34*0.621371)</f>
+        <f t="shared" ref="S34:S65" si="2">_xlfn.FLOOR.MATH(F34*0.621371)</f>
         <v>18</v>
       </c>
       <c r="T34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -2588,11 +2588,11 @@
         <v>0</v>
       </c>
       <c r="S35">
-        <f>_xlfn.FLOOR.MATH(F35*0.621371)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="T35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -2642,11 +2642,11 @@
         <v>0</v>
       </c>
       <c r="S36">
-        <f>_xlfn.FLOOR.MATH(F36*0.621371)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="T36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -2696,11 +2696,11 @@
         <v>0</v>
       </c>
       <c r="S37">
-        <f>_xlfn.FLOOR.MATH(F37*0.621371)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="T37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -2750,11 +2750,11 @@
         <v>0</v>
       </c>
       <c r="S38">
-        <f>_xlfn.FLOOR.MATH(F38*0.621371)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="T38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -2804,11 +2804,11 @@
         <v>0</v>
       </c>
       <c r="S39">
-        <f>_xlfn.FLOOR.MATH(F39*0.621371)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="T39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -2862,11 +2862,11 @@
         <v>0</v>
       </c>
       <c r="S40">
-        <f>_xlfn.FLOOR.MATH(F40*0.621371)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="T40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -2916,11 +2916,11 @@
         <v>0</v>
       </c>
       <c r="S41">
-        <f>_xlfn.FLOOR.MATH(F41*0.621371)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="T41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -2970,11 +2970,11 @@
         <v>0</v>
       </c>
       <c r="S42">
-        <f>_xlfn.FLOOR.MATH(F42*0.621371)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="T42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -3024,11 +3024,11 @@
         <v>0</v>
       </c>
       <c r="S43">
-        <f>_xlfn.FLOOR.MATH(F43*0.621371)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="T43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -3078,11 +3078,11 @@
         <v>0</v>
       </c>
       <c r="S44">
-        <f>_xlfn.FLOOR.MATH(F44*0.621371)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="T44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -3132,11 +3132,11 @@
         <v>0</v>
       </c>
       <c r="S45">
-        <f>_xlfn.FLOOR.MATH(F45*0.621371)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="T45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -3186,11 +3186,11 @@
         <v>0</v>
       </c>
       <c r="S46">
-        <f>_xlfn.FLOOR.MATH(F46*0.621371)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="T46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -3240,11 +3240,11 @@
         <v>0</v>
       </c>
       <c r="S47">
-        <f>_xlfn.FLOOR.MATH(F47*0.621371)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="T47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -3294,11 +3294,11 @@
         <v>0</v>
       </c>
       <c r="S48">
-        <f>_xlfn.FLOOR.MATH(F48*0.621371)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="T48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -3352,11 +3352,11 @@
         <v>0</v>
       </c>
       <c r="S49">
-        <f>_xlfn.FLOOR.MATH(F49*0.621371)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="T49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -3406,11 +3406,11 @@
         <v>0</v>
       </c>
       <c r="S50">
-        <f>_xlfn.FLOOR.MATH(F50*0.621371)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="T50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -3460,11 +3460,11 @@
         <v>0</v>
       </c>
       <c r="S51">
-        <f>_xlfn.FLOOR.MATH(F51*0.621371)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="T51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -3514,11 +3514,11 @@
         <v>0</v>
       </c>
       <c r="S52">
-        <f>_xlfn.FLOOR.MATH(F52*0.621371)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="T52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -3568,11 +3568,11 @@
         <v>0</v>
       </c>
       <c r="S53">
-        <f>_xlfn.FLOOR.MATH(F53*0.621371)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="T53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -3622,11 +3622,11 @@
         <v>0</v>
       </c>
       <c r="S54">
-        <f>_xlfn.FLOOR.MATH(F54*0.621371)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="T54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -3676,11 +3676,11 @@
         <v>0</v>
       </c>
       <c r="S55">
-        <f>_xlfn.FLOOR.MATH(F55*0.621371)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="T55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -3730,11 +3730,11 @@
         <v>0</v>
       </c>
       <c r="S56">
-        <f>_xlfn.FLOOR.MATH(F56*0.621371)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="T56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -3784,11 +3784,11 @@
         <v>0</v>
       </c>
       <c r="S57">
-        <f>_xlfn.FLOOR.MATH(F57*0.621371)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="T57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -3844,11 +3844,11 @@
         <v>0</v>
       </c>
       <c r="S58">
-        <f>_xlfn.FLOOR.MATH(F58*0.621371)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="T58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -3899,11 +3899,11 @@
         <v>0</v>
       </c>
       <c r="S59">
-        <f>_xlfn.FLOOR.MATH(F59*0.621371)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="T59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -3953,11 +3953,11 @@
         <v>0</v>
       </c>
       <c r="S60">
-        <f>_xlfn.FLOOR.MATH(F60*0.621371)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="T60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -4007,11 +4007,11 @@
         <v>0</v>
       </c>
       <c r="S61">
-        <f>_xlfn.FLOOR.MATH(F61*0.621371)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="T61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -4061,11 +4061,11 @@
         <v>0</v>
       </c>
       <c r="S62">
-        <f>_xlfn.FLOOR.MATH(F62*0.621371)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="T62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -4119,11 +4119,11 @@
         <v>0</v>
       </c>
       <c r="S63">
-        <f>_xlfn.FLOOR.MATH(F63*0.621371)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="T63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -4173,11 +4173,11 @@
         <v>0</v>
       </c>
       <c r="S64">
-        <f>_xlfn.FLOOR.MATH(F64*0.621371)</f>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="T64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -4227,11 +4227,11 @@
         <v>0</v>
       </c>
       <c r="S65">
-        <f>_xlfn.FLOOR.MATH(F65*0.621371)</f>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="T65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -4285,11 +4285,11 @@
         <v>0</v>
       </c>
       <c r="S66">
-        <f>_xlfn.FLOOR.MATH(F66*0.621371)</f>
+        <f t="shared" ref="S66:S97" si="3">_xlfn.FLOOR.MATH(F66*0.621371)</f>
         <v>43</v>
       </c>
       <c r="T66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>218.72199999999998</v>
       </c>
     </row>
@@ -4339,11 +4339,11 @@
         <v>0</v>
       </c>
       <c r="S67">
-        <f>_xlfn.FLOOR.MATH(F67*0.621371)</f>
+        <f t="shared" si="3"/>
         <v>43</v>
       </c>
       <c r="T67">
-        <f t="shared" ref="T67:T130" si="1">D67 * 1.09361</f>
+        <f t="shared" ref="T67:T130" si="4">D67 * 1.09361</f>
         <v>218.72199999999998</v>
       </c>
     </row>
@@ -4393,11 +4393,11 @@
         <v>0</v>
       </c>
       <c r="S68">
-        <f>_xlfn.FLOOR.MATH(F68*0.621371)</f>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="T68">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -4447,11 +4447,11 @@
         <v>0</v>
       </c>
       <c r="S69">
-        <f>_xlfn.FLOOR.MATH(F69*0.621371)</f>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="T69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -4501,11 +4501,11 @@
         <v>0</v>
       </c>
       <c r="S70">
-        <f>_xlfn.FLOOR.MATH(F70*0.621371)</f>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="T70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -4555,11 +4555,11 @@
         <v>0</v>
       </c>
       <c r="S71">
-        <f>_xlfn.FLOOR.MATH(F71*0.621371)</f>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="T71">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -4609,11 +4609,11 @@
         <v>0</v>
       </c>
       <c r="S72">
-        <f>_xlfn.FLOOR.MATH(F72*0.621371)</f>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="T72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -4663,11 +4663,11 @@
         <v>0</v>
       </c>
       <c r="S73">
-        <f>_xlfn.FLOOR.MATH(F73*0.621371)</f>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="T73">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -4721,11 +4721,11 @@
         <v>0</v>
       </c>
       <c r="S74">
-        <f>_xlfn.FLOOR.MATH(F74*0.621371)</f>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="T74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -4775,11 +4775,11 @@
         <v>0</v>
       </c>
       <c r="S75">
-        <f>_xlfn.FLOOR.MATH(F75*0.621371)</f>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="T75">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -4829,11 +4829,11 @@
         <v>0</v>
       </c>
       <c r="S76">
-        <f>_xlfn.FLOOR.MATH(F76*0.621371)</f>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="T76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -4885,11 +4885,11 @@
         <v>0</v>
       </c>
       <c r="S77">
-        <f>_xlfn.FLOOR.MATH(F77*0.621371)</f>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="T77">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -4943,11 +4943,11 @@
         <v>0</v>
       </c>
       <c r="S78">
-        <f>_xlfn.FLOOR.MATH(F78*0.621371)</f>
+        <f t="shared" si="3"/>
         <v>43</v>
       </c>
       <c r="T78">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>328.08299999999997</v>
       </c>
     </row>
@@ -4997,11 +4997,11 @@
         <v>0</v>
       </c>
       <c r="S79">
-        <f>_xlfn.FLOOR.MATH(F79*0.621371)</f>
+        <f t="shared" si="3"/>
         <v>43</v>
       </c>
       <c r="T79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>328.08299999999997</v>
       </c>
     </row>
@@ -5051,11 +5051,11 @@
         <v>0</v>
       </c>
       <c r="S80">
-        <f>_xlfn.FLOOR.MATH(F80*0.621371)</f>
+        <f t="shared" si="3"/>
         <v>43</v>
       </c>
       <c r="T80">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>328.08299999999997</v>
       </c>
     </row>
@@ -5105,11 +5105,11 @@
         <v>0</v>
       </c>
       <c r="S81">
-        <f>_xlfn.FLOOR.MATH(F81*0.621371)</f>
+        <f t="shared" si="3"/>
         <v>43</v>
       </c>
       <c r="T81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>328.08299999999997</v>
       </c>
     </row>
@@ -5159,11 +5159,11 @@
         <v>0</v>
       </c>
       <c r="S82">
-        <f>_xlfn.FLOOR.MATH(F82*0.621371)</f>
+        <f t="shared" si="3"/>
         <v>43</v>
       </c>
       <c r="T82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>328.08299999999997</v>
       </c>
     </row>
@@ -5213,11 +5213,11 @@
         <v>0</v>
       </c>
       <c r="S83">
-        <f>_xlfn.FLOOR.MATH(F83*0.621371)</f>
+        <f t="shared" si="3"/>
         <v>43</v>
       </c>
       <c r="T83">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>328.08299999999997</v>
       </c>
     </row>
@@ -5267,11 +5267,11 @@
         <v>0</v>
       </c>
       <c r="S84">
-        <f>_xlfn.FLOOR.MATH(F84*0.621371)</f>
+        <f t="shared" si="3"/>
         <v>43</v>
       </c>
       <c r="T84">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>328.08299999999997</v>
       </c>
     </row>
@@ -5321,11 +5321,11 @@
         <v>0</v>
       </c>
       <c r="S85">
-        <f>_xlfn.FLOOR.MATH(F85*0.621371)</f>
+        <f t="shared" si="3"/>
         <v>43</v>
       </c>
       <c r="T85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>328.08299999999997</v>
       </c>
     </row>
@@ -5377,11 +5377,11 @@
         <v>0</v>
       </c>
       <c r="S86">
-        <f>_xlfn.FLOOR.MATH(F86*0.621371)</f>
+        <f t="shared" si="3"/>
         <v>43</v>
       </c>
       <c r="T86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>328.08299999999997</v>
       </c>
     </row>
@@ -5431,11 +5431,11 @@
         <v>0</v>
       </c>
       <c r="S87">
-        <f>_xlfn.FLOOR.MATH(F87*0.621371)</f>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="T87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -5485,11 +5485,11 @@
         <v>0</v>
       </c>
       <c r="S88">
-        <f>_xlfn.FLOOR.MATH(F88*0.621371)</f>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="T88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>94.706625999999986</v>
       </c>
     </row>
@@ -5543,11 +5543,11 @@
         <v>0</v>
       </c>
       <c r="S89">
-        <f>_xlfn.FLOOR.MATH(F89*0.621371)</f>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="T89">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -5597,11 +5597,11 @@
         <v>0</v>
       </c>
       <c r="S90">
-        <f>_xlfn.FLOOR.MATH(F90*0.621371)</f>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="T90">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>82.020749999999992</v>
       </c>
     </row>
@@ -5651,11 +5651,11 @@
         <v>0</v>
       </c>
       <c r="S91">
-        <f>_xlfn.FLOOR.MATH(F91*0.621371)</f>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="T91">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>82.020749999999992</v>
       </c>
     </row>
@@ -5705,11 +5705,11 @@
         <v>0</v>
       </c>
       <c r="S92">
-        <f>_xlfn.FLOOR.MATH(F92*0.621371)</f>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="T92">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>82.020749999999992</v>
       </c>
     </row>
@@ -5759,11 +5759,11 @@
         <v>0</v>
       </c>
       <c r="S93">
-        <f>_xlfn.FLOOR.MATH(F93*0.621371)</f>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="T93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>82.020749999999992</v>
       </c>
     </row>
@@ -5813,11 +5813,11 @@
         <v>0</v>
       </c>
       <c r="S94">
-        <f>_xlfn.FLOOR.MATH(F94*0.621371)</f>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="T94">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>82.020749999999992</v>
       </c>
     </row>
@@ -5867,11 +5867,11 @@
         <v>0</v>
       </c>
       <c r="S95">
-        <f>_xlfn.FLOOR.MATH(F95*0.621371)</f>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="T95">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>82.020749999999992</v>
       </c>
     </row>
@@ -5921,11 +5921,11 @@
         <v>0</v>
       </c>
       <c r="S96">
-        <f>_xlfn.FLOOR.MATH(F96*0.621371)</f>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="T96">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>82.020749999999992</v>
       </c>
     </row>
@@ -5979,11 +5979,11 @@
         <v>0</v>
       </c>
       <c r="S97">
-        <f>_xlfn.FLOOR.MATH(F97*0.621371)</f>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="T97">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>82.020749999999992</v>
       </c>
     </row>
@@ -6033,11 +6033,11 @@
         <v>0</v>
       </c>
       <c r="S98">
-        <f>_xlfn.FLOOR.MATH(F98*0.621371)</f>
+        <f t="shared" ref="S98:S129" si="5">_xlfn.FLOOR.MATH(F98*0.621371)</f>
         <v>15</v>
       </c>
       <c r="T98">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>82.020749999999992</v>
       </c>
     </row>
@@ -6087,11 +6087,11 @@
         <v>0</v>
       </c>
       <c r="S99">
-        <f>_xlfn.FLOOR.MATH(F99*0.621371)</f>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="T99">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>82.020749999999992</v>
       </c>
     </row>
@@ -6141,11 +6141,11 @@
         <v>0</v>
       </c>
       <c r="S100">
-        <f>_xlfn.FLOOR.MATH(F100*0.621371)</f>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="T100">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>82.020749999999992</v>
       </c>
     </row>
@@ -6195,11 +6195,11 @@
         <v>0</v>
       </c>
       <c r="S101">
-        <f>_xlfn.FLOOR.MATH(F101*0.621371)</f>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="T101">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>82.020749999999992</v>
       </c>
     </row>
@@ -6249,11 +6249,11 @@
         <v>0</v>
       </c>
       <c r="S102">
-        <f>_xlfn.FLOOR.MATH(F102*0.621371)</f>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="T102">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>38.276350000000001</v>
       </c>
     </row>
@@ -6303,11 +6303,11 @@
         <v>0</v>
       </c>
       <c r="S103">
-        <f>_xlfn.FLOOR.MATH(F103*0.621371)</f>
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
       <c r="T103">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -6357,11 +6357,11 @@
         <v>0</v>
       </c>
       <c r="S104">
-        <f>_xlfn.FLOOR.MATH(F104*0.621371)</f>
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
       <c r="T104">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -6411,11 +6411,11 @@
         <v>0</v>
       </c>
       <c r="S105">
-        <f>_xlfn.FLOOR.MATH(F105*0.621371)</f>
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
       <c r="T105">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>87.488799999999998</v>
       </c>
     </row>
@@ -6469,11 +6469,11 @@
         <v>0</v>
       </c>
       <c r="S106">
-        <f>_xlfn.FLOOR.MATH(F106*0.621371)</f>
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
       <c r="T106">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -6523,11 +6523,11 @@
         <v>0</v>
       </c>
       <c r="S107">
-        <f>_xlfn.FLOOR.MATH(F107*0.621371)</f>
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
       <c r="T107">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -6577,11 +6577,11 @@
         <v>0</v>
       </c>
       <c r="S108">
-        <f>_xlfn.FLOOR.MATH(F108*0.621371)</f>
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
       <c r="T108">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>98.424899999999994</v>
       </c>
     </row>
@@ -6631,11 +6631,11 @@
         <v>0</v>
       </c>
       <c r="S109">
-        <f>_xlfn.FLOOR.MATH(F109*0.621371)</f>
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
       <c r="T109">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -6685,11 +6685,11 @@
         <v>0</v>
       </c>
       <c r="S110">
-        <f>_xlfn.FLOOR.MATH(F110*0.621371)</f>
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
       <c r="T110">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -6739,11 +6739,11 @@
         <v>0</v>
       </c>
       <c r="S111">
-        <f>_xlfn.FLOOR.MATH(F111*0.621371)</f>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="T111">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -6793,11 +6793,11 @@
         <v>0</v>
       </c>
       <c r="S112">
-        <f>_xlfn.FLOOR.MATH(F112*0.621371)</f>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="T112">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -6847,11 +6847,11 @@
         <v>0</v>
       </c>
       <c r="S113">
-        <f>_xlfn.FLOOR.MATH(F113*0.621371)</f>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="T113">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -6901,11 +6901,11 @@
         <v>0</v>
       </c>
       <c r="S114">
-        <f>_xlfn.FLOOR.MATH(F114*0.621371)</f>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="T114">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -6959,11 +6959,11 @@
         <v>0</v>
       </c>
       <c r="S115">
-        <f>_xlfn.FLOOR.MATH(F115*0.621371)</f>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="T115">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>177.16481999999999</v>
       </c>
     </row>
@@ -7013,11 +7013,11 @@
         <v>0</v>
       </c>
       <c r="S116">
-        <f>_xlfn.FLOOR.MATH(F116*0.621371)</f>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="T116">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -7067,11 +7067,11 @@
         <v>0</v>
       </c>
       <c r="S117">
-        <f>_xlfn.FLOOR.MATH(F117*0.621371)</f>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="T117">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>109.36099999999999</v>
       </c>
     </row>
@@ -7121,11 +7121,11 @@
         <v>0</v>
       </c>
       <c r="S118">
-        <f>_xlfn.FLOOR.MATH(F118*0.621371)</f>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="T118">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -7175,11 +7175,11 @@
         <v>0</v>
       </c>
       <c r="S119">
-        <f>_xlfn.FLOOR.MATH(F119*0.621371)</f>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="T119">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -7229,11 +7229,11 @@
         <v>0</v>
       </c>
       <c r="S120">
-        <f>_xlfn.FLOOR.MATH(F120*0.621371)</f>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="T120">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>43.744399999999999</v>
       </c>
     </row>
@@ -7283,11 +7283,11 @@
         <v>0</v>
       </c>
       <c r="S121">
-        <f>_xlfn.FLOOR.MATH(F121*0.621371)</f>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="T121">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -7337,11 +7337,11 @@
         <v>0</v>
       </c>
       <c r="S122">
-        <f>_xlfn.FLOOR.MATH(F122*0.621371)</f>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="T122">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -7391,11 +7391,11 @@
         <v>0</v>
       </c>
       <c r="S123">
-        <f>_xlfn.FLOOR.MATH(F123*0.621371)</f>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="T123">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -7449,11 +7449,11 @@
         <v>0</v>
       </c>
       <c r="S124">
-        <f>_xlfn.FLOOR.MATH(F124*0.621371)</f>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="T124">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -7503,11 +7503,11 @@
         <v>0</v>
       </c>
       <c r="S125">
-        <f>_xlfn.FLOOR.MATH(F125*0.621371)</f>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="T125">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -7557,11 +7557,11 @@
         <v>0</v>
       </c>
       <c r="S126">
-        <f>_xlfn.FLOOR.MATH(F126*0.621371)</f>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="T126">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -7611,11 +7611,11 @@
         <v>0</v>
       </c>
       <c r="S127">
-        <f>_xlfn.FLOOR.MATH(F127*0.621371)</f>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="T127">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -7665,11 +7665,11 @@
         <v>0</v>
       </c>
       <c r="S128">
-        <f>_xlfn.FLOOR.MATH(F128*0.621371)</f>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="T128">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -7719,11 +7719,11 @@
         <v>0</v>
       </c>
       <c r="S129">
-        <f>_xlfn.FLOOR.MATH(F129*0.621371)</f>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="T129">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -7773,11 +7773,11 @@
         <v>0</v>
       </c>
       <c r="S130">
-        <f>_xlfn.FLOOR.MATH(F130*0.621371)</f>
+        <f t="shared" ref="S130:S151" si="6">_xlfn.FLOOR.MATH(F130*0.621371)</f>
         <v>12</v>
       </c>
       <c r="T130">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -7827,11 +7827,11 @@
         <v>0</v>
       </c>
       <c r="S131">
-        <f>_xlfn.FLOOR.MATH(F131*0.621371)</f>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="T131">
-        <f t="shared" ref="T131:T151" si="2">D131 * 1.09361</f>
+        <f t="shared" ref="T131:T151" si="7">D131 * 1.09361</f>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -7881,11 +7881,11 @@
         <v>0</v>
       </c>
       <c r="S132">
-        <f>_xlfn.FLOOR.MATH(F132*0.621371)</f>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="T132">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -7939,11 +7939,11 @@
         <v>0</v>
       </c>
       <c r="S133">
-        <f>_xlfn.FLOOR.MATH(F133*0.621371)</f>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="T133">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -7993,11 +7993,11 @@
         <v>0</v>
       </c>
       <c r="S134">
-        <f>_xlfn.FLOOR.MATH(F134*0.621371)</f>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="T134">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -8047,11 +8047,11 @@
         <v>0</v>
       </c>
       <c r="S135">
-        <f>_xlfn.FLOOR.MATH(F135*0.621371)</f>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="T135">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -8101,11 +8101,11 @@
         <v>0</v>
       </c>
       <c r="S136">
-        <f>_xlfn.FLOOR.MATH(F136*0.621371)</f>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="T136">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -8155,11 +8155,11 @@
         <v>0</v>
       </c>
       <c r="S137">
-        <f>_xlfn.FLOOR.MATH(F137*0.621371)</f>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="T137">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -8209,11 +8209,11 @@
         <v>0</v>
       </c>
       <c r="S138">
-        <f>_xlfn.FLOOR.MATH(F138*0.621371)</f>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="T138">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -8263,11 +8263,11 @@
         <v>0</v>
       </c>
       <c r="S139">
-        <f>_xlfn.FLOOR.MATH(F139*0.621371)</f>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="T139">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -8317,11 +8317,11 @@
         <v>0</v>
       </c>
       <c r="S140">
-        <f>_xlfn.FLOOR.MATH(F140*0.621371)</f>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="T140">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -8371,11 +8371,11 @@
         <v>0</v>
       </c>
       <c r="S141">
-        <f>_xlfn.FLOOR.MATH(F141*0.621371)</f>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="T141">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -8429,11 +8429,11 @@
         <v>0</v>
       </c>
       <c r="S142">
-        <f>_xlfn.FLOOR.MATH(F142*0.621371)</f>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="T142">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -8483,11 +8483,11 @@
         <v>0</v>
       </c>
       <c r="S143">
-        <f>_xlfn.FLOOR.MATH(F143*0.621371)</f>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="T143">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -8537,11 +8537,11 @@
         <v>0</v>
       </c>
       <c r="S144">
-        <f>_xlfn.FLOOR.MATH(F144*0.621371)</f>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="T144">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -8591,11 +8591,11 @@
         <v>0</v>
       </c>
       <c r="S145">
-        <f>_xlfn.FLOOR.MATH(F145*0.621371)</f>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="T145">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -8645,11 +8645,11 @@
         <v>0</v>
       </c>
       <c r="S146">
-        <f>_xlfn.FLOOR.MATH(F146*0.621371)</f>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="T146">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -8699,11 +8699,11 @@
         <v>0</v>
       </c>
       <c r="S147">
-        <f>_xlfn.FLOOR.MATH(F147*0.621371)</f>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="T147">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -8753,11 +8753,11 @@
         <v>0</v>
       </c>
       <c r="S148">
-        <f>_xlfn.FLOOR.MATH(F148*0.621371)</f>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="T148">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -8807,11 +8807,11 @@
         <v>0</v>
       </c>
       <c r="S149">
-        <f>_xlfn.FLOOR.MATH(F149*0.621371)</f>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="T149">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>201.22424000000001</v>
       </c>
     </row>
@@ -8861,11 +8861,11 @@
         <v>0</v>
       </c>
       <c r="S150">
-        <f>_xlfn.FLOOR.MATH(F150*0.621371)</f>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="T150">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>43.744399999999999</v>
       </c>
     </row>
@@ -8917,11 +8917,11 @@
         <v>0</v>
       </c>
       <c r="S151">
-        <f>_xlfn.FLOOR.MATH(F151*0.621371)</f>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="T151">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>38.276350000000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed ui tables, lists still need work
</commit_message>
<xml_diff>
--- a/src/Track/TrackModel/GreenLine_Layout.xlsx
+++ b/src/Track/TrackModel/GreenLine_Layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cjame\Documents\ECE1140ChooChoo\src\Track\TrackModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA70F400-791D-4721-AFC1-AF13C9A34895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7FD375F-DD42-48DA-B02D-B5229ABBF670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2700" windowWidth="29040" windowHeight="15840" xr2:uid="{85290365-C1DC-46B7-8A8F-B8FE040B733E}"/>
   </bookViews>
@@ -642,7 +642,7 @@
   <dimension ref="A1:T151"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
-      <selection activeCell="U6" sqref="U6"/>
+      <selection activeCell="Q110" sqref="Q110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added note in excel about switch exit
</commit_message>
<xml_diff>
--- a/src/Track/TrackModel/GreenLine_Layout.xlsx
+++ b/src/Track/TrackModel/GreenLine_Layout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aeone\Documents\ECE1140ChooChoo\src\Track\TrackModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB21C716-6F80-4E82-9830-5228AB87C6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871962D1-91EE-4376-8696-15B94404946B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{85290365-C1DC-46B7-8A8F-B8FE040B733E}"/>
+    <workbookView xWindow="1920" yWindow="1656" windowWidth="17280" windowHeight="11304" xr2:uid="{85290365-C1DC-46B7-8A8F-B8FE040B733E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,6 +34,40 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Connor M</author>
+  </authors>
+  <commentList>
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{AB36E1A5-B427-40C4-84DD-4DFE4F4A8164}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Connor M:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+For switch exit column, if the corresponding block has a value in the column it is a switch exit and the corresponding value in the column is the switch entrance</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -265,7 +299,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,6 +322,19 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -663,11 +710,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{521756E0-942E-44A0-8B9B-C1C5C2AAFFBA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{521756E0-942E-44A0-8B9B-C1C5C2AAFFBA}">
   <dimension ref="A1:U151"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
-      <selection activeCell="K86" sqref="K86"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8982,6 +9029,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Excel edits made to add both yard blocks
</commit_message>
<xml_diff>
--- a/src/Track/TrackModel/GreenLine_Layout.xlsx
+++ b/src/Track/TrackModel/GreenLine_Layout.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aeone\Documents\ECE1140ChooChoo\src\Track\TrackModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5C206C-0D8C-4628-922D-2EE9B585A0D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DF292D-7AE2-4221-AE48-70914005EA20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{85290365-C1DC-46B7-8A8F-B8FE040B733E}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="83">
   <si>
     <t>Section</t>
   </si>
@@ -210,9 +210,6 @@
     <t>Exit Blocks</t>
   </si>
   <si>
-    <t>57-Yard, 57-58</t>
-  </si>
-  <si>
     <t>Speed Limit (MPH)</t>
   </si>
   <si>
@@ -249,9 +246,6 @@
     <t>28-29,28-150</t>
   </si>
   <si>
-    <t>63-Yard, 63-62</t>
-  </si>
-  <si>
     <t>77-76,77-101</t>
   </si>
   <si>
@@ -280,6 +274,18 @@
   </si>
   <si>
     <t>K62</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>57-152, 57-58</t>
+  </si>
+  <si>
+    <t>63-151, 63-62</t>
   </si>
 </sst>
 </file>
@@ -685,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{521756E0-942E-44A0-8B9B-C1C5C2AAFFBA}">
-  <dimension ref="A1:V151"/>
+  <dimension ref="A1:V153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="74" workbookViewId="0">
-      <selection activeCell="O74" sqref="O74"/>
+    <sheetView tabSelected="1" topLeftCell="E132" zoomScale="74" workbookViewId="0">
+      <selection activeCell="K156" sqref="K156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -748,7 +754,7 @@
         <v>6</v>
       </c>
       <c r="L1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>11</v>
@@ -757,10 +763,10 @@
         <v>12</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>13</v>
@@ -775,10 +781,10 @@
         <v>56</v>
       </c>
       <c r="U1" t="s">
+        <v>57</v>
+      </c>
+      <c r="V1" t="s">
         <v>58</v>
-      </c>
-      <c r="V1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
@@ -810,7 +816,7 @@
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M2" s="4">
         <v>1</v>
@@ -1447,7 +1453,7 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="L13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M13" s="4">
         <v>1</v>
@@ -1459,7 +1465,7 @@
         <v>1</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="Q13" s="4">
         <v>0</v>
@@ -1508,7 +1514,7 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M14" s="4">
         <v>0</v>
@@ -2373,7 +2379,7 @@
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M29" s="4">
         <v>0</v>
@@ -2433,7 +2439,7 @@
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
       <c r="L30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M30" s="4">
         <v>1</v>
@@ -2445,7 +2451,7 @@
         <v>1</v>
       </c>
       <c r="P30" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="Q30" s="4">
         <v>0</v>
@@ -4049,7 +4055,7 @@
         <v>1</v>
       </c>
       <c r="K58" s="4" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="M58" s="4">
         <v>0</v>
@@ -4108,7 +4114,7 @@
       <c r="I59" s="4"/>
       <c r="J59" s="4"/>
       <c r="L59" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M59" s="4">
         <v>1</v>
@@ -4120,7 +4126,7 @@
         <v>1</v>
       </c>
       <c r="P59" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q59" s="4">
         <v>0</v>
@@ -4340,7 +4346,7 @@
       <c r="I63" s="4"/>
       <c r="J63" s="4"/>
       <c r="L63" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M63" s="4">
         <v>1</v>
@@ -4352,7 +4358,7 @@
         <v>1</v>
       </c>
       <c r="P63" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q63" s="4">
         <v>0</v>
@@ -4401,7 +4407,7 @@
       <c r="I64" s="4"/>
       <c r="J64" s="4"/>
       <c r="K64" s="4" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="M64" s="4">
         <v>0</v>
@@ -5152,7 +5158,7 @@
       <c r="I77" s="4"/>
       <c r="J77" s="4"/>
       <c r="L77" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M77" s="4">
         <v>1</v>
@@ -5215,7 +5221,7 @@
         <v>2</v>
       </c>
       <c r="K78" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M78" s="4">
         <v>0</v>
@@ -5673,7 +5679,7 @@
       <c r="I86" s="4"/>
       <c r="J86" s="4"/>
       <c r="K86" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="M86" s="4">
         <v>0</v>
@@ -5733,7 +5739,7 @@
       <c r="J87" s="4"/>
       <c r="K87" s="4"/>
       <c r="L87" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M87" s="4">
         <v>1</v>
@@ -5745,7 +5751,7 @@
         <v>1</v>
       </c>
       <c r="P87" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Q87" s="4">
         <v>0</v>
@@ -6544,7 +6550,7 @@
       <c r="J101" s="4"/>
       <c r="K101" s="4"/>
       <c r="L101" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M101" s="4">
         <v>1</v>
@@ -6604,7 +6610,7 @@
       <c r="J102" s="4"/>
       <c r="K102" s="4"/>
       <c r="L102" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M102" s="4">
         <v>1</v>
@@ -6616,7 +6622,7 @@
         <v>1</v>
       </c>
       <c r="P102" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Q102" s="4">
         <v>0</v>
@@ -8296,11 +8302,11 @@
         <v>0</v>
       </c>
       <c r="U131">
-        <f t="shared" ref="U131:U151" si="4">F131*0.621371</f>
+        <f t="shared" ref="U131:U153" si="4">F131*0.621371</f>
         <v>12.42742</v>
       </c>
       <c r="V131">
-        <f t="shared" ref="V131:V151" si="5">D131 * 1.09361</f>
+        <f t="shared" ref="V131:V153" si="5">D131 * 1.09361</f>
         <v>54.680499999999995</v>
       </c>
     </row>
@@ -9422,7 +9428,7 @@
       <c r="J151" s="4"/>
       <c r="K151" s="4"/>
       <c r="L151" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M151" s="4">
         <v>1</v>
@@ -9453,6 +9459,116 @@
       <c r="V151">
         <f t="shared" si="5"/>
         <v>38.276350000000001</v>
+      </c>
+    </row>
+    <row r="152" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B152" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C152" s="4">
+        <v>151</v>
+      </c>
+      <c r="D152" s="4">
+        <v>100</v>
+      </c>
+      <c r="E152" s="4">
+        <v>0</v>
+      </c>
+      <c r="F152" s="4">
+        <v>15</v>
+      </c>
+      <c r="G152" s="4">
+        <v>0</v>
+      </c>
+      <c r="H152" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="L152" t="s">
+        <v>64</v>
+      </c>
+      <c r="M152" s="4">
+        <v>1</v>
+      </c>
+      <c r="N152" s="4">
+        <v>0</v>
+      </c>
+      <c r="O152" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q152" s="4">
+        <v>0</v>
+      </c>
+      <c r="R152" s="5">
+        <v>24</v>
+      </c>
+      <c r="S152" s="4">
+        <v>2</v>
+      </c>
+      <c r="T152">
+        <v>0</v>
+      </c>
+      <c r="U152">
+        <f t="shared" si="4"/>
+        <v>9.3205650000000002</v>
+      </c>
+      <c r="V152">
+        <f t="shared" si="5"/>
+        <v>109.36099999999999</v>
+      </c>
+    </row>
+    <row r="153" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B153" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C153" s="4">
+        <v>152</v>
+      </c>
+      <c r="D153" s="4">
+        <v>100</v>
+      </c>
+      <c r="E153" s="4">
+        <v>0</v>
+      </c>
+      <c r="F153" s="4">
+        <v>15</v>
+      </c>
+      <c r="G153" s="4">
+        <v>0</v>
+      </c>
+      <c r="H153" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="L153" t="s">
+        <v>63</v>
+      </c>
+      <c r="M153" s="4">
+        <v>1</v>
+      </c>
+      <c r="N153" s="4">
+        <v>0</v>
+      </c>
+      <c r="O153" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q153" s="4">
+        <v>0</v>
+      </c>
+      <c r="R153" s="5">
+        <v>24</v>
+      </c>
+      <c r="S153" s="4">
+        <v>2</v>
+      </c>
+      <c r="T153">
+        <v>0</v>
+      </c>
+      <c r="U153">
+        <f t="shared" si="4"/>
+        <v>9.3205650000000002</v>
+      </c>
+      <c r="V153">
+        <f t="shared" si="5"/>
+        <v>109.36099999999999</v>
       </c>
     </row>
   </sheetData>
@@ -9462,10 +9578,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88653644-AF3E-4625-A5A7-2FF88949AA53}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9478,7 +9594,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -9686,6 +9802,22 @@
         <v>39</v>
       </c>
       <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed track model backend to deal with yard blocks
</commit_message>
<xml_diff>
--- a/src/Track/TrackModel/GreenLine_Layout.xlsx
+++ b/src/Track/TrackModel/GreenLine_Layout.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aeone\Documents\ECE1140ChooChoo\src\Track\TrackModel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connor Marsh\Desktop\Trains\ECE1140ChooChoo\src\Track\TrackModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DF292D-7AE2-4221-AE48-70914005EA20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64AE713A-14E1-48B8-BE9A-1CBEFE6C6008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{85290365-C1DC-46B7-8A8F-B8FE040B733E}"/>
+    <workbookView xWindow="2814" yWindow="978" windowWidth="16902" windowHeight="11262" xr2:uid="{85290365-C1DC-46B7-8A8F-B8FE040B733E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="82">
   <si>
     <t>Section</t>
   </si>
@@ -274,9 +274,6 @@
   </si>
   <si>
     <t>K62</t>
-  </si>
-  <si>
-    <t>$</t>
   </si>
   <si>
     <t>y</t>
@@ -693,33 +690,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{521756E0-942E-44A0-8B9B-C1C5C2AAFFBA}">
   <dimension ref="A1:V153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E132" zoomScale="74" workbookViewId="0">
-      <selection activeCell="K156" sqref="K156"/>
+    <sheetView tabSelected="1" topLeftCell="A131" zoomScale="74" workbookViewId="0">
+      <selection activeCell="I148" sqref="I148"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.20703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1015625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.77734375" customWidth="1"/>
-    <col min="13" max="13" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.21875" customWidth="1"/>
-    <col min="15" max="15" width="8.21875" customWidth="1"/>
-    <col min="16" max="16" width="12.44140625" customWidth="1"/>
+    <col min="7" max="7" width="9.5234375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.20703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5234375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.89453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7890625" customWidth="1"/>
+    <col min="13" max="13" width="5.41796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.20703125" customWidth="1"/>
+    <col min="15" max="15" width="8.20703125" customWidth="1"/>
+    <col min="16" max="16" width="12.41796875" customWidth="1"/>
     <col min="17" max="17" width="13" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.20703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.3125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.5234375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.41796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -787,7 +784,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
@@ -849,7 +846,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
         <v>4</v>
@@ -910,7 +907,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
         <v>4</v>
@@ -967,7 +964,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
@@ -1024,7 +1021,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
         <v>9</v>
@@ -1081,7 +1078,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
         <v>9</v>
@@ -1138,7 +1135,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
         <v>10</v>
@@ -1195,7 +1192,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
         <v>10</v>
@@ -1252,7 +1249,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
         <v>10</v>
@@ -1313,7 +1310,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
         <v>10</v>
@@ -1370,7 +1367,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="4"/>
       <c r="B12" s="4" t="s">
         <v>10</v>
@@ -1427,7 +1424,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="4"/>
       <c r="B13" s="4" t="s">
         <v>10</v>
@@ -1488,7 +1485,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
         <v>17</v>
@@ -1547,7 +1544,7 @@
         <v>164.04149999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
         <v>17</v>
@@ -1604,7 +1601,7 @@
         <v>164.04149999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="4"/>
       <c r="B16" s="4" t="s">
         <v>17</v>
@@ -1661,7 +1658,7 @@
         <v>164.04149999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="4"/>
       <c r="B17" s="4" t="s">
         <v>17</v>
@@ -1722,7 +1719,7 @@
         <v>164.04149999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="4"/>
       <c r="B18" s="4" t="s">
         <v>18</v>
@@ -1779,7 +1776,7 @@
         <v>164.04149999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="4"/>
       <c r="B19" s="4" t="s">
         <v>18</v>
@@ -1836,7 +1833,7 @@
         <v>164.04149999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="4"/>
       <c r="B20" s="4" t="s">
         <v>18</v>
@@ -1893,7 +1890,7 @@
         <v>164.04149999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="4"/>
       <c r="B21" s="4" t="s">
         <v>18</v>
@@ -1950,7 +1947,7 @@
         <v>164.04149999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="4"/>
       <c r="B22" s="4" t="s">
         <v>19</v>
@@ -2007,7 +2004,7 @@
         <v>328.08299999999997</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="4"/>
       <c r="B23" s="4" t="s">
         <v>19</v>
@@ -2068,7 +2065,7 @@
         <v>328.08299999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="4"/>
       <c r="B24" s="4" t="s">
         <v>19</v>
@@ -2125,7 +2122,7 @@
         <v>328.08299999999997</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="4"/>
       <c r="B25" s="4" t="s">
         <v>19</v>
@@ -2182,7 +2179,7 @@
         <v>328.08299999999997</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="4"/>
       <c r="B26" s="4" t="s">
         <v>19</v>
@@ -2239,7 +2236,7 @@
         <v>218.72199999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="4"/>
       <c r="B27" s="4" t="s">
         <v>19</v>
@@ -2296,7 +2293,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="4"/>
       <c r="B28" s="4" t="s">
         <v>19</v>
@@ -2353,7 +2350,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="4"/>
       <c r="B29" s="4" t="s">
         <v>19</v>
@@ -2412,7 +2409,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="4"/>
       <c r="B30" s="4" t="s">
         <v>20</v>
@@ -2474,7 +2471,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="4"/>
       <c r="B31" s="4" t="s">
         <v>20</v>
@@ -2531,7 +2528,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="4"/>
       <c r="B32" s="4" t="s">
         <v>20</v>
@@ -2592,7 +2589,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="4"/>
       <c r="B33" s="4" t="s">
         <v>20</v>
@@ -2649,7 +2646,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="4"/>
       <c r="B34" s="4" t="s">
         <v>21</v>
@@ -2706,7 +2703,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="4"/>
       <c r="B35" s="4" t="s">
         <v>21</v>
@@ -2763,7 +2760,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="4"/>
       <c r="B36" s="4" t="s">
         <v>21</v>
@@ -2820,7 +2817,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="4"/>
       <c r="B37" s="4" t="s">
         <v>22</v>
@@ -2877,7 +2874,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="4"/>
       <c r="B38" s="4" t="s">
         <v>22</v>
@@ -2934,7 +2931,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="4"/>
       <c r="B39" s="4" t="s">
         <v>22</v>
@@ -2991,7 +2988,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="4"/>
       <c r="B40" s="4" t="s">
         <v>22</v>
@@ -3052,7 +3049,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="4"/>
       <c r="B41" s="4" t="s">
         <v>22</v>
@@ -3109,7 +3106,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="4"/>
       <c r="B42" s="4" t="s">
         <v>22</v>
@@ -3166,7 +3163,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="4"/>
       <c r="B43" s="4" t="s">
         <v>22</v>
@@ -3223,7 +3220,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="4"/>
       <c r="B44" s="4" t="s">
         <v>22</v>
@@ -3280,7 +3277,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="4"/>
       <c r="B45" s="4" t="s">
         <v>22</v>
@@ -3337,7 +3334,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="4"/>
       <c r="B46" s="4" t="s">
         <v>22</v>
@@ -3394,7 +3391,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="4"/>
       <c r="B47" s="4" t="s">
         <v>22</v>
@@ -3451,7 +3448,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="4"/>
       <c r="B48" s="4" t="s">
         <v>22</v>
@@ -3508,7 +3505,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="4"/>
       <c r="B49" s="4" t="s">
         <v>22</v>
@@ -3569,7 +3566,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="4"/>
       <c r="B50" s="4" t="s">
         <v>22</v>
@@ -3626,7 +3623,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="4"/>
       <c r="B51" s="4" t="s">
         <v>22</v>
@@ -3683,7 +3680,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="4"/>
       <c r="B52" s="4" t="s">
         <v>22</v>
@@ -3740,7 +3737,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="4"/>
       <c r="B53" s="4" t="s">
         <v>22</v>
@@ -3797,7 +3794,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="4"/>
       <c r="B54" s="4" t="s">
         <v>22</v>
@@ -3854,7 +3851,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="4"/>
       <c r="B55" s="4" t="s">
         <v>22</v>
@@ -3911,7 +3908,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="4"/>
       <c r="B56" s="4" t="s">
         <v>22</v>
@@ -3968,7 +3965,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="4"/>
       <c r="B57" s="4" t="s">
         <v>22</v>
@@ -4025,7 +4022,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="4"/>
       <c r="B58" s="4" t="s">
         <v>22</v>
@@ -4055,7 +4052,7 @@
         <v>1</v>
       </c>
       <c r="K58" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M58" s="4">
         <v>0</v>
@@ -4088,7 +4085,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="4"/>
       <c r="B59" s="4" t="s">
         <v>23</v>
@@ -4149,7 +4146,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="4"/>
       <c r="B60" s="4" t="s">
         <v>23</v>
@@ -4206,7 +4203,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="4"/>
       <c r="B61" s="4" t="s">
         <v>23</v>
@@ -4263,7 +4260,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="4"/>
       <c r="B62" s="4" t="s">
         <v>23</v>
@@ -4320,7 +4317,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="4"/>
       <c r="B63" s="4" t="s">
         <v>23</v>
@@ -4381,7 +4378,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="4"/>
       <c r="B64" s="4" t="s">
         <v>24</v>
@@ -4407,7 +4404,7 @@
       <c r="I64" s="4"/>
       <c r="J64" s="4"/>
       <c r="K64" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M64" s="4">
         <v>0</v>
@@ -4440,7 +4437,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="4"/>
       <c r="B65" s="4" t="s">
         <v>24</v>
@@ -4497,7 +4494,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="4"/>
       <c r="B66" s="4" t="s">
         <v>24</v>
@@ -4558,7 +4555,7 @@
         <v>218.72199999999998</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="4"/>
       <c r="B67" s="4" t="s">
         <v>24</v>
@@ -4615,7 +4612,7 @@
         <v>218.72199999999998</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="4"/>
       <c r="B68" s="4" t="s">
         <v>24</v>
@@ -4672,7 +4669,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="4"/>
       <c r="B69" s="4" t="s">
         <v>24</v>
@@ -4729,7 +4726,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="4"/>
       <c r="B70" s="4" t="s">
         <v>25</v>
@@ -4786,7 +4783,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="4"/>
       <c r="B71" s="4" t="s">
         <v>25</v>
@@ -4843,7 +4840,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="4"/>
       <c r="B72" s="4" t="s">
         <v>25</v>
@@ -4900,7 +4897,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="4"/>
       <c r="B73" s="4" t="s">
         <v>25</v>
@@ -4957,7 +4954,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="4"/>
       <c r="B74" s="4" t="s">
         <v>25</v>
@@ -5018,7 +5015,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="4"/>
       <c r="B75" s="4" t="s">
         <v>26</v>
@@ -5075,7 +5072,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="4"/>
       <c r="B76" s="4" t="s">
         <v>26</v>
@@ -5132,7 +5129,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="4"/>
       <c r="B77" s="4" t="s">
         <v>26</v>
@@ -5191,7 +5188,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="4"/>
       <c r="B78" s="4" t="s">
         <v>27</v>
@@ -5254,7 +5251,7 @@
         <v>328.08299999999997</v>
       </c>
     </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="4"/>
       <c r="B79" s="4" t="s">
         <v>27</v>
@@ -5311,7 +5308,7 @@
         <v>328.08299999999997</v>
       </c>
     </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="4"/>
       <c r="B80" s="4" t="s">
         <v>27</v>
@@ -5368,7 +5365,7 @@
         <v>328.08299999999997</v>
       </c>
     </row>
-    <row r="81" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="4"/>
       <c r="B81" s="4" t="s">
         <v>27</v>
@@ -5425,7 +5422,7 @@
         <v>328.08299999999997</v>
       </c>
     </row>
-    <row r="82" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="4"/>
       <c r="B82" s="4" t="s">
         <v>27</v>
@@ -5482,7 +5479,7 @@
         <v>328.08299999999997</v>
       </c>
     </row>
-    <row r="83" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="4"/>
       <c r="B83" s="4" t="s">
         <v>27</v>
@@ -5539,7 +5536,7 @@
         <v>328.08299999999997</v>
       </c>
     </row>
-    <row r="84" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="4"/>
       <c r="B84" s="4" t="s">
         <v>27</v>
@@ -5596,7 +5593,7 @@
         <v>328.08299999999997</v>
       </c>
     </row>
-    <row r="85" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="4"/>
       <c r="B85" s="4" t="s">
         <v>27</v>
@@ -5653,7 +5650,7 @@
         <v>328.08299999999997</v>
       </c>
     </row>
-    <row r="86" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="4"/>
       <c r="B86" s="4" t="s">
         <v>27</v>
@@ -5712,7 +5709,7 @@
         <v>328.08299999999997</v>
       </c>
     </row>
-    <row r="87" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="4"/>
       <c r="B87" s="4" t="s">
         <v>28</v>
@@ -5774,7 +5771,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="88" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="4"/>
       <c r="B88" s="4" t="s">
         <v>28</v>
@@ -5831,7 +5828,7 @@
         <v>94.706625999999986</v>
       </c>
     </row>
-    <row r="89" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="4"/>
       <c r="B89" s="4" t="s">
         <v>28</v>
@@ -5892,7 +5889,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="90" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="4"/>
       <c r="B90" s="4" t="s">
         <v>29</v>
@@ -5949,7 +5946,7 @@
         <v>82.020749999999992</v>
       </c>
     </row>
-    <row r="91" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="4"/>
       <c r="B91" s="4" t="s">
         <v>29</v>
@@ -6006,7 +6003,7 @@
         <v>82.020749999999992</v>
       </c>
     </row>
-    <row r="92" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="4"/>
       <c r="B92" s="4" t="s">
         <v>29</v>
@@ -6063,7 +6060,7 @@
         <v>82.020749999999992</v>
       </c>
     </row>
-    <row r="93" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="4"/>
       <c r="B93" s="4" t="s">
         <v>29</v>
@@ -6120,7 +6117,7 @@
         <v>82.020749999999992</v>
       </c>
     </row>
-    <row r="94" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="4"/>
       <c r="B94" s="4" t="s">
         <v>29</v>
@@ -6177,7 +6174,7 @@
         <v>82.020749999999992</v>
       </c>
     </row>
-    <row r="95" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="4"/>
       <c r="B95" s="4" t="s">
         <v>29</v>
@@ -6234,7 +6231,7 @@
         <v>82.020749999999992</v>
       </c>
     </row>
-    <row r="96" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="4"/>
       <c r="B96" s="4" t="s">
         <v>29</v>
@@ -6291,7 +6288,7 @@
         <v>82.020749999999992</v>
       </c>
     </row>
-    <row r="97" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="4"/>
       <c r="B97" s="4" t="s">
         <v>29</v>
@@ -6352,7 +6349,7 @@
         <v>82.020749999999992</v>
       </c>
     </row>
-    <row r="98" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="4"/>
       <c r="B98" s="4" t="s">
         <v>29</v>
@@ -6409,7 +6406,7 @@
         <v>82.020749999999992</v>
       </c>
     </row>
-    <row r="99" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="4"/>
       <c r="B99" s="4" t="s">
         <v>30</v>
@@ -6466,7 +6463,7 @@
         <v>82.020749999999992</v>
       </c>
     </row>
-    <row r="100" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="4"/>
       <c r="B100" s="4" t="s">
         <v>30</v>
@@ -6523,7 +6520,7 @@
         <v>82.020749999999992</v>
       </c>
     </row>
-    <row r="101" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="4"/>
       <c r="B101" s="4" t="s">
         <v>30</v>
@@ -6583,7 +6580,7 @@
         <v>82.020749999999992</v>
       </c>
     </row>
-    <row r="102" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="4"/>
       <c r="B102" s="4" t="s">
         <v>31</v>
@@ -6645,7 +6642,7 @@
         <v>38.276350000000001</v>
       </c>
     </row>
-    <row r="103" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="4"/>
       <c r="B103" s="4" t="s">
         <v>32</v>
@@ -6702,7 +6699,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="104" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="4"/>
       <c r="B104" s="4" t="s">
         <v>32</v>
@@ -6759,7 +6756,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="105" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="4"/>
       <c r="B105" s="4" t="s">
         <v>32</v>
@@ -6816,7 +6813,7 @@
         <v>87.488799999999998</v>
       </c>
     </row>
-    <row r="106" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="4"/>
       <c r="B106" s="4" t="s">
         <v>33</v>
@@ -6877,7 +6874,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="107" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="4"/>
       <c r="B107" s="4" t="s">
         <v>33</v>
@@ -6934,7 +6931,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="108" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="4"/>
       <c r="B108" s="4" t="s">
         <v>33</v>
@@ -6991,7 +6988,7 @@
         <v>98.424899999999994</v>
       </c>
     </row>
-    <row r="109" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="4"/>
       <c r="B109" s="4" t="s">
         <v>33</v>
@@ -7048,7 +7045,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="110" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="4"/>
       <c r="B110" s="4" t="s">
         <v>33</v>
@@ -7105,7 +7102,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="111" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="4"/>
       <c r="B111" s="4" t="s">
         <v>34</v>
@@ -7162,7 +7159,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="112" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="4"/>
       <c r="B112" s="4" t="s">
         <v>34</v>
@@ -7219,7 +7216,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="113" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="4"/>
       <c r="B113" s="4" t="s">
         <v>34</v>
@@ -7276,7 +7273,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="114" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="4"/>
       <c r="B114" s="4" t="s">
         <v>34</v>
@@ -7333,7 +7330,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="115" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="4"/>
       <c r="B115" s="4" t="s">
         <v>34</v>
@@ -7394,7 +7391,7 @@
         <v>177.16481999999999</v>
       </c>
     </row>
-    <row r="116" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="4"/>
       <c r="B116" s="4" t="s">
         <v>34</v>
@@ -7451,7 +7448,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="117" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="4"/>
       <c r="B117" s="4" t="s">
         <v>34</v>
@@ -7508,7 +7505,7 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="118" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="4"/>
       <c r="B118" s="4" t="s">
         <v>35</v>
@@ -7565,7 +7562,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="119" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="4"/>
       <c r="B119" s="4" t="s">
         <v>35</v>
@@ -7622,7 +7619,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="120" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="4"/>
       <c r="B120" s="4" t="s">
         <v>35</v>
@@ -7679,7 +7676,7 @@
         <v>43.744399999999999</v>
       </c>
     </row>
-    <row r="121" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="4"/>
       <c r="B121" s="4" t="s">
         <v>35</v>
@@ -7736,7 +7733,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="122" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="4"/>
       <c r="B122" s="4" t="s">
         <v>35</v>
@@ -7793,7 +7790,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="123" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="4"/>
       <c r="B123" s="4" t="s">
         <v>36</v>
@@ -7850,7 +7847,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="124" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="4"/>
       <c r="B124" s="4" t="s">
         <v>36</v>
@@ -7911,7 +7908,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="125" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="4"/>
       <c r="B125" s="4" t="s">
         <v>36</v>
@@ -7968,7 +7965,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="126" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="4"/>
       <c r="B126" s="4" t="s">
         <v>36</v>
@@ -8025,7 +8022,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="127" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="4"/>
       <c r="B127" s="4" t="s">
         <v>36</v>
@@ -8082,7 +8079,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="128" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="4"/>
       <c r="B128" s="4" t="s">
         <v>36</v>
@@ -8139,7 +8136,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="129" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="4"/>
       <c r="B129" s="4" t="s">
         <v>36</v>
@@ -8196,7 +8193,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="130" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="4"/>
       <c r="B130" s="4" t="s">
         <v>36</v>
@@ -8253,7 +8250,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="131" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="4"/>
       <c r="B131" s="4" t="s">
         <v>36</v>
@@ -8310,7 +8307,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="132" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="4"/>
       <c r="B132" s="4" t="s">
         <v>36</v>
@@ -8367,7 +8364,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="133" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="4"/>
       <c r="B133" s="4" t="s">
         <v>36</v>
@@ -8428,7 +8425,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="134" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="4"/>
       <c r="B134" s="4" t="s">
         <v>36</v>
@@ -8485,7 +8482,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="135" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="4"/>
       <c r="B135" s="4" t="s">
         <v>36</v>
@@ -8542,7 +8539,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="136" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="4"/>
       <c r="B136" s="4" t="s">
         <v>36</v>
@@ -8599,7 +8596,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="137" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="4"/>
       <c r="B137" s="4" t="s">
         <v>36</v>
@@ -8656,7 +8653,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="138" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="4"/>
       <c r="B138" s="4" t="s">
         <v>36</v>
@@ -8713,7 +8710,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="139" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="4"/>
       <c r="B139" s="4" t="s">
         <v>36</v>
@@ -8770,7 +8767,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="140" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="4"/>
       <c r="B140" s="4" t="s">
         <v>36</v>
@@ -8827,7 +8824,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="141" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="4"/>
       <c r="B141" s="4" t="s">
         <v>36</v>
@@ -8884,7 +8881,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="142" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="4"/>
       <c r="B142" s="4" t="s">
         <v>36</v>
@@ -8945,7 +8942,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="143" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="4"/>
       <c r="B143" s="4" t="s">
         <v>36</v>
@@ -9002,7 +8999,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="144" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="4"/>
       <c r="B144" s="4" t="s">
         <v>36</v>
@@ -9059,7 +9056,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="145" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="4"/>
       <c r="B145" s="4" t="s">
         <v>37</v>
@@ -9116,7 +9113,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="146" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="4"/>
       <c r="B146" s="4" t="s">
         <v>37</v>
@@ -9173,7 +9170,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="147" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="4"/>
       <c r="B147" s="4" t="s">
         <v>37</v>
@@ -9230,7 +9227,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="148" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="4"/>
       <c r="B148" s="4" t="s">
         <v>38</v>
@@ -9287,7 +9284,7 @@
         <v>54.680499999999995</v>
       </c>
     </row>
-    <row r="149" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="4"/>
       <c r="B149" s="4" t="s">
         <v>38</v>
@@ -9344,7 +9341,7 @@
         <v>201.22424000000001</v>
       </c>
     </row>
-    <row r="150" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="4"/>
       <c r="B150" s="4" t="s">
         <v>38</v>
@@ -9401,7 +9398,7 @@
         <v>43.744399999999999</v>
       </c>
     </row>
-    <row r="151" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="4"/>
       <c r="B151" s="4" t="s">
         <v>39</v>
@@ -9461,7 +9458,7 @@
         <v>38.276350000000001</v>
       </c>
     </row>
-    <row r="152" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="B152" s="4" t="s">
         <v>79</v>
       </c>
@@ -9516,9 +9513,9 @@
         <v>109.36099999999999</v>
       </c>
     </row>
-    <row r="153" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="B153" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C153" s="4">
         <v>152</v>
@@ -9578,18 +9575,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88653644-AF3E-4625-A5A7-2FF88949AA53}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.3125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -9597,7 +9594,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -9605,7 +9602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -9613,7 +9610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -9621,7 +9618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -9629,7 +9626,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -9637,7 +9634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -9645,7 +9642,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -9653,7 +9650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -9661,7 +9658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -9669,7 +9666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -9677,7 +9674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -9685,7 +9682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -9693,7 +9690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -9701,7 +9698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -9709,7 +9706,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -9717,7 +9714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -9725,7 +9722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -9733,7 +9730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -9741,7 +9738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -9749,7 +9746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -9757,7 +9754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -9765,7 +9762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -9773,7 +9770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -9781,7 +9778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -9789,7 +9786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -9797,7 +9794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -9805,19 +9802,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>79</v>
       </c>
       <c r="B28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>80</v>
-      </c>
-      <c r="B29">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
hopefully fixed overlapping territory? Probably very unstable
</commit_message>
<xml_diff>
--- a/src/Track/TrackModel/GreenLine_Layout.xlsx
+++ b/src/Track/TrackModel/GreenLine_Layout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aeone\Documents\ECE1140ChooChoo\src\Track\TrackModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DF292D-7AE2-4221-AE48-70914005EA20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BED2A9D-41D9-4ED2-9C4D-D9819E5549EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{85290365-C1DC-46B7-8A8F-B8FE040B733E}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{85290365-C1DC-46B7-8A8F-B8FE040B733E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="84">
   <si>
     <t>Section</t>
   </si>
@@ -276,9 +276,6 @@
     <t>K62</t>
   </si>
   <si>
-    <t>$</t>
-  </si>
-  <si>
     <t>y</t>
   </si>
   <si>
@@ -286,6 +283,12 @@
   </si>
   <si>
     <t>63-151, 63-62</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>2,3</t>
   </si>
 </sst>
 </file>
@@ -693,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{521756E0-942E-44A0-8B9B-C1C5C2AAFFBA}">
   <dimension ref="A1:V153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E132" zoomScale="74" workbookViewId="0">
-      <selection activeCell="K156" sqref="K156"/>
+    <sheetView tabSelected="1" topLeftCell="E130" zoomScale="74" workbookViewId="0">
+      <selection activeCell="A136" sqref="A136:XFD136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2862,8 +2865,8 @@
       <c r="R37" s="5">
         <v>6</v>
       </c>
-      <c r="S37">
-        <v>2</v>
+      <c r="S37" t="s">
+        <v>82</v>
       </c>
       <c r="T37">
         <v>0</v>
@@ -2919,8 +2922,8 @@
       <c r="R38" s="5">
         <v>6</v>
       </c>
-      <c r="S38">
-        <v>2</v>
+      <c r="S38" t="s">
+        <v>82</v>
       </c>
       <c r="T38">
         <v>0</v>
@@ -2959,7 +2962,6 @@
       </c>
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
       <c r="M39" s="4">
         <v>0</v>
       </c>
@@ -2976,8 +2978,8 @@
       <c r="R39" s="5">
         <v>6</v>
       </c>
-      <c r="S39">
-        <v>2</v>
+      <c r="S39" t="s">
+        <v>82</v>
       </c>
       <c r="T39">
         <v>0</v>
@@ -4055,7 +4057,7 @@
         <v>1</v>
       </c>
       <c r="K58" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M58" s="4">
         <v>0</v>
@@ -4407,7 +4409,7 @@
       <c r="I64" s="4"/>
       <c r="J64" s="4"/>
       <c r="K64" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M64" s="4">
         <v>0</v>
@@ -4771,8 +4773,8 @@
       <c r="R70" s="5">
         <v>9</v>
       </c>
-      <c r="S70">
-        <v>3</v>
+      <c r="S70" t="s">
+        <v>83</v>
       </c>
       <c r="T70">
         <v>0</v>
@@ -4828,8 +4830,8 @@
       <c r="R71" s="5">
         <v>9</v>
       </c>
-      <c r="S71">
-        <v>3</v>
+      <c r="S71" t="s">
+        <v>83</v>
       </c>
       <c r="T71">
         <v>0</v>
@@ -4885,8 +4887,8 @@
       <c r="R72" s="5">
         <v>9</v>
       </c>
-      <c r="S72">
-        <v>3</v>
+      <c r="S72" t="s">
+        <v>83</v>
       </c>
       <c r="T72">
         <v>0</v>
@@ -7147,8 +7149,8 @@
       <c r="R111" s="5">
         <v>12</v>
       </c>
-      <c r="S111">
-        <v>2</v>
+      <c r="S111" t="s">
+        <v>83</v>
       </c>
       <c r="T111">
         <v>0</v>
@@ -7204,8 +7206,8 @@
       <c r="R112" s="5">
         <v>12</v>
       </c>
-      <c r="S112">
-        <v>2</v>
+      <c r="S112" t="s">
+        <v>83</v>
       </c>
       <c r="T112">
         <v>0</v>
@@ -7261,8 +7263,8 @@
       <c r="R113" s="5">
         <v>12</v>
       </c>
-      <c r="S113">
-        <v>2</v>
+      <c r="S113" t="s">
+        <v>83</v>
       </c>
       <c r="T113">
         <v>0</v>
@@ -8584,8 +8586,8 @@
       <c r="R136" s="5">
         <v>9</v>
       </c>
-      <c r="S136">
-        <v>1</v>
+      <c r="S136" t="s">
+        <v>82</v>
       </c>
       <c r="T136">
         <v>0</v>
@@ -8641,8 +8643,8 @@
       <c r="R137" s="5">
         <v>9</v>
       </c>
-      <c r="S137">
-        <v>1</v>
+      <c r="S137" t="s">
+        <v>82</v>
       </c>
       <c r="T137">
         <v>0</v>
@@ -8698,8 +8700,8 @@
       <c r="R138" s="5">
         <v>9</v>
       </c>
-      <c r="S138">
-        <v>1</v>
+      <c r="S138" t="s">
+        <v>82</v>
       </c>
       <c r="T138">
         <v>0</v>
@@ -9518,7 +9520,7 @@
     </row>
     <row r="153" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B153" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C153" s="4">
         <v>152</v>
@@ -9578,10 +9580,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88653644-AF3E-4625-A5A7-2FF88949AA53}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9813,14 +9815,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>80</v>
-      </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Exit block can be sent to wayside now
</commit_message>
<xml_diff>
--- a/src/Track/TrackModel/GreenLine_Layout.xlsx
+++ b/src/Track/TrackModel/GreenLine_Layout.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cjame\Documents\ECE1140ChooChoo\src\Track\TrackModel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aeone\Documents\ECE1140ChooChoo\src\Track\TrackModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52F1996-EB88-4377-90CE-CB95DC997355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C1CFB8-7F5D-4A19-8DFD-A54BE9DCF583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2700" windowWidth="29040" windowHeight="15840" xr2:uid="{85290365-C1DC-46B7-8A8F-B8FE040B733E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{85290365-C1DC-46B7-8A8F-B8FE040B733E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -696,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{521756E0-942E-44A0-8B9B-C1C5C2AAFFBA}">
   <dimension ref="A1:V153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="74" workbookViewId="0">
-      <selection activeCell="C110" sqref="C110"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="74" workbookViewId="0">
+      <selection activeCell="U116" sqref="U116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2812,7 +2812,7 @@
         <v>1</v>
       </c>
       <c r="T36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U36">
         <f t="shared" si="0"/>
@@ -4720,7 +4720,7 @@
         <v>2</v>
       </c>
       <c r="T69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U69">
         <f t="shared" si="2"/>
@@ -7096,7 +7096,7 @@
         <v>3</v>
       </c>
       <c r="T110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U110">
         <f t="shared" si="2"/>
@@ -9562,7 +9562,7 @@
         <v>2</v>
       </c>
       <c r="T153">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U153">
         <f t="shared" si="4"/>

</xml_diff>

<commit_message>
Made small change to track_data_class making global red line auto import
</commit_message>
<xml_diff>
--- a/src/Track/TrackModel/GreenLine_Layout.xlsx
+++ b/src/Track/TrackModel/GreenLine_Layout.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cjame\Documents\ECE1140ChooChoo\src\Track\TrackModel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aeone\Documents\ECE1140ChooChoo\src\Track\TrackModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52F1996-EB88-4377-90CE-CB95DC997355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C1CFB8-7F5D-4A19-8DFD-A54BE9DCF583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2700" windowWidth="29040" windowHeight="15840" xr2:uid="{85290365-C1DC-46B7-8A8F-B8FE040B733E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{85290365-C1DC-46B7-8A8F-B8FE040B733E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -696,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{521756E0-942E-44A0-8B9B-C1C5C2AAFFBA}">
   <dimension ref="A1:V153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="74" workbookViewId="0">
-      <selection activeCell="C110" sqref="C110"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="74" workbookViewId="0">
+      <selection activeCell="U116" sqref="U116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2812,7 +2812,7 @@
         <v>1</v>
       </c>
       <c r="T36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U36">
         <f t="shared" si="0"/>
@@ -4720,7 +4720,7 @@
         <v>2</v>
       </c>
       <c r="T69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U69">
         <f t="shared" si="2"/>
@@ -7096,7 +7096,7 @@
         <v>3</v>
       </c>
       <c r="T110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U110">
         <f t="shared" si="2"/>
@@ -9562,7 +9562,7 @@
         <v>2</v>
       </c>
       <c r="T153">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U153">
         <f t="shared" si="4"/>

</xml_diff>

<commit_message>
added traversal times to block structs
</commit_message>
<xml_diff>
--- a/src/Track/TrackModel/GreenLine_Layout.xlsx
+++ b/src/Track/TrackModel/GreenLine_Layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aeone\Documents\ECE1140ChooChoo\src\Track\TrackModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C1CFB8-7F5D-4A19-8DFD-A54BE9DCF583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415E75F4-F29F-4EF8-93B5-ED3742AFB875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{85290365-C1DC-46B7-8A8F-B8FE040B733E}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="85">
   <si>
     <t>Section</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>2,3</t>
+  </si>
+  <si>
+    <t>Traversal Time</t>
   </si>
 </sst>
 </file>
@@ -694,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{521756E0-942E-44A0-8B9B-C1C5C2AAFFBA}">
-  <dimension ref="A1:V153"/>
+  <dimension ref="A1:W153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="74" workbookViewId="0">
-      <selection activeCell="U116" sqref="U116"/>
+    <sheetView tabSelected="1" topLeftCell="J19" zoomScale="74" workbookViewId="0">
+      <selection activeCell="W152" sqref="W152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -720,9 +723,10 @@
     <col min="19" max="19" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -789,8 +793,11 @@
       <c r="V1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
@@ -851,8 +858,11 @@
         <f>D2 * 1.09361</f>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
         <v>4</v>
@@ -912,8 +922,11 @@
         <f t="shared" ref="V3:V66" si="1">D3 * 1.09361</f>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
         <v>4</v>
@@ -969,8 +982,11 @@
         <f t="shared" si="1"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
@@ -1026,8 +1042,11 @@
         <f t="shared" si="1"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
         <v>9</v>
@@ -1083,8 +1102,11 @@
         <f t="shared" si="1"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
         <v>9</v>
@@ -1140,8 +1162,11 @@
         <f t="shared" si="1"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
         <v>10</v>
@@ -1197,8 +1222,11 @@
         <f t="shared" si="1"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
         <v>10</v>
@@ -1254,8 +1282,11 @@
         <f t="shared" si="1"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
         <v>10</v>
@@ -1315,8 +1346,11 @@
         <f t="shared" si="1"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
         <v>10</v>
@@ -1372,8 +1406,11 @@
         <f t="shared" si="1"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="4" t="s">
         <v>10</v>
@@ -1429,8 +1466,11 @@
         <f t="shared" si="1"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="4" t="s">
         <v>10</v>
@@ -1490,8 +1530,11 @@
         <f t="shared" si="1"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
         <v>17</v>
@@ -1549,8 +1592,11 @@
         <f t="shared" si="1"/>
         <v>164.04149999999998</v>
       </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W14">
+        <v>7.7142857142857153</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
         <v>17</v>
@@ -1606,8 +1652,11 @@
         <f t="shared" si="1"/>
         <v>164.04149999999998</v>
       </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W15">
+        <v>7.7142857142857153</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="4" t="s">
         <v>17</v>
@@ -1663,8 +1712,11 @@
         <f t="shared" si="1"/>
         <v>164.04149999999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W16">
+        <v>7.7142857142857153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="4" t="s">
         <v>17</v>
@@ -1724,8 +1776,11 @@
         <f t="shared" si="1"/>
         <v>164.04149999999998</v>
       </c>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W17">
+        <v>7.7142857142857153</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4" t="s">
         <v>18</v>
@@ -1781,8 +1836,11 @@
         <f t="shared" si="1"/>
         <v>164.04149999999998</v>
       </c>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="4" t="s">
         <v>18</v>
@@ -1838,8 +1896,11 @@
         <f t="shared" si="1"/>
         <v>164.04149999999998</v>
       </c>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4" t="s">
         <v>18</v>
@@ -1895,8 +1956,11 @@
         <f t="shared" si="1"/>
         <v>164.04149999999998</v>
       </c>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W20">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="4" t="s">
         <v>18</v>
@@ -1952,8 +2016,11 @@
         <f t="shared" si="1"/>
         <v>164.04149999999998</v>
       </c>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="4" t="s">
         <v>19</v>
@@ -2009,8 +2076,11 @@
         <f t="shared" si="1"/>
         <v>328.08299999999997</v>
       </c>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W22">
+        <v>15.428571428571431</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4" t="s">
         <v>19</v>
@@ -2070,8 +2140,11 @@
         <f t="shared" si="1"/>
         <v>328.08299999999997</v>
       </c>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W23">
+        <v>15.428571428571431</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4" t="s">
         <v>19</v>
@@ -2127,8 +2200,11 @@
         <f t="shared" si="1"/>
         <v>328.08299999999997</v>
       </c>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W24">
+        <v>15.428571428571431</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="4" t="s">
         <v>19</v>
@@ -2184,8 +2260,11 @@
         <f t="shared" si="1"/>
         <v>328.08299999999997</v>
       </c>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W25">
+        <v>15.428571428571431</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4" t="s">
         <v>19</v>
@@ -2241,8 +2320,11 @@
         <f t="shared" si="1"/>
         <v>218.72199999999998</v>
       </c>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W26">
+        <v>10.285714285714286</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="4" t="s">
         <v>19</v>
@@ -2298,8 +2380,11 @@
         <f t="shared" si="1"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W27">
+        <v>5.1428571428571432</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="4" t="s">
         <v>19</v>
@@ -2355,8 +2440,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="4" t="s">
         <v>19</v>
@@ -2414,8 +2502,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="4" t="s">
         <v>20</v>
@@ -2476,8 +2567,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="4" t="s">
         <v>20</v>
@@ -2533,8 +2627,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="4" t="s">
         <v>20</v>
@@ -2594,8 +2691,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W32">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="4" t="s">
         <v>20</v>
@@ -2651,8 +2751,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4" t="s">
         <v>21</v>
@@ -2708,8 +2811,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W34">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4" t="s">
         <v>21</v>
@@ -2765,8 +2871,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="4" t="s">
         <v>21</v>
@@ -2822,8 +2931,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W36">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="4" t="s">
         <v>22</v>
@@ -2879,8 +2991,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W37">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="4" t="s">
         <v>22</v>
@@ -2936,8 +3051,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W38">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="4" t="s">
         <v>22</v>
@@ -2992,8 +3110,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W39">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
       <c r="B40" s="4" t="s">
         <v>22</v>
@@ -3053,8 +3174,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="4" t="s">
         <v>22</v>
@@ -3110,8 +3234,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W41">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
       <c r="B42" s="4" t="s">
         <v>22</v>
@@ -3167,8 +3294,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W42">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
       <c r="B43" s="4" t="s">
         <v>22</v>
@@ -3224,8 +3354,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W43">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
       <c r="B44" s="4" t="s">
         <v>22</v>
@@ -3281,8 +3414,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W44">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A45" s="4"/>
       <c r="B45" s="4" t="s">
         <v>22</v>
@@ -3338,8 +3474,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A46" s="4"/>
       <c r="B46" s="4" t="s">
         <v>22</v>
@@ -3395,8 +3534,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W46">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A47" s="4"/>
       <c r="B47" s="4" t="s">
         <v>22</v>
@@ -3452,8 +3594,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W47">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A48" s="4"/>
       <c r="B48" s="4" t="s">
         <v>22</v>
@@ -3509,8 +3654,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W48">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A49" s="4"/>
       <c r="B49" s="4" t="s">
         <v>22</v>
@@ -3570,8 +3718,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W49">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A50" s="4"/>
       <c r="B50" s="4" t="s">
         <v>22</v>
@@ -3627,8 +3778,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W50">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A51" s="4"/>
       <c r="B51" s="4" t="s">
         <v>22</v>
@@ -3684,8 +3838,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W51">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A52" s="4"/>
       <c r="B52" s="4" t="s">
         <v>22</v>
@@ -3741,8 +3898,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W52">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A53" s="4"/>
       <c r="B53" s="4" t="s">
         <v>22</v>
@@ -3798,8 +3958,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W53">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A54" s="4"/>
       <c r="B54" s="4" t="s">
         <v>22</v>
@@ -3855,8 +4018,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W54">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A55" s="4"/>
       <c r="B55" s="4" t="s">
         <v>22</v>
@@ -3912,8 +4078,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W55">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A56" s="4"/>
       <c r="B56" s="4" t="s">
         <v>22</v>
@@ -3969,8 +4138,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W56">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A57" s="4"/>
       <c r="B57" s="4" t="s">
         <v>22</v>
@@ -4026,8 +4198,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W57">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A58" s="4"/>
       <c r="B58" s="4" t="s">
         <v>22</v>
@@ -4089,8 +4264,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W58">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A59" s="4"/>
       <c r="B59" s="4" t="s">
         <v>23</v>
@@ -4150,8 +4328,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
       <c r="B60" s="4" t="s">
         <v>23</v>
@@ -4207,8 +4388,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W60">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A61" s="4"/>
       <c r="B61" s="4" t="s">
         <v>23</v>
@@ -4264,8 +4448,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W61">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A62" s="4"/>
       <c r="B62" s="4" t="s">
         <v>23</v>
@@ -4321,8 +4508,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W62">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A63" s="4"/>
       <c r="B63" s="4" t="s">
         <v>23</v>
@@ -4382,8 +4572,11 @@
         <f t="shared" si="1"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W63">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A64" s="4"/>
       <c r="B64" s="4" t="s">
         <v>24</v>
@@ -4441,8 +4634,11 @@
         <f t="shared" si="1"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W64">
+        <v>5.1428571428571432</v>
+      </c>
+    </row>
+    <row r="65" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A65" s="4"/>
       <c r="B65" s="4" t="s">
         <v>24</v>
@@ -4498,8 +4694,11 @@
         <f t="shared" si="1"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W65">
+        <v>5.1428571428571432</v>
+      </c>
+    </row>
+    <row r="66" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A66" s="4"/>
       <c r="B66" s="4" t="s">
         <v>24</v>
@@ -4559,8 +4758,11 @@
         <f t="shared" si="1"/>
         <v>218.72199999999998</v>
       </c>
-    </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W66">
+        <v>10.285714285714286</v>
+      </c>
+    </row>
+    <row r="67" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A67" s="4"/>
       <c r="B67" s="4" t="s">
         <v>24</v>
@@ -4616,8 +4818,11 @@
         <f t="shared" ref="V67:V130" si="3">D67 * 1.09361</f>
         <v>218.72199999999998</v>
       </c>
-    </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W67">
+        <v>10.285714285714286</v>
+      </c>
+    </row>
+    <row r="68" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A68" s="4"/>
       <c r="B68" s="4" t="s">
         <v>24</v>
@@ -4673,8 +4878,11 @@
         <f t="shared" si="3"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W68">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A69" s="4"/>
       <c r="B69" s="4" t="s">
         <v>24</v>
@@ -4730,8 +4938,11 @@
         <f t="shared" si="3"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W69">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A70" s="4"/>
       <c r="B70" s="4" t="s">
         <v>25</v>
@@ -4787,8 +4998,11 @@
         <f t="shared" si="3"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W70">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A71" s="4"/>
       <c r="B71" s="4" t="s">
         <v>25</v>
@@ -4844,8 +5058,11 @@
         <f t="shared" si="3"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W71">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A72" s="4"/>
       <c r="B72" s="4" t="s">
         <v>25</v>
@@ -4901,8 +5118,11 @@
         <f t="shared" si="3"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W72">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A73" s="4"/>
       <c r="B73" s="4" t="s">
         <v>25</v>
@@ -4958,8 +5178,11 @@
         <f t="shared" si="3"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W73">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A74" s="4"/>
       <c r="B74" s="4" t="s">
         <v>25</v>
@@ -5019,8 +5242,11 @@
         <f t="shared" si="3"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W74">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A75" s="4"/>
       <c r="B75" s="4" t="s">
         <v>26</v>
@@ -5076,8 +5302,11 @@
         <f t="shared" si="3"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W75">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A76" s="4"/>
       <c r="B76" s="4" t="s">
         <v>26</v>
@@ -5133,8 +5362,11 @@
         <f t="shared" si="3"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W76">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A77" s="4"/>
       <c r="B77" s="4" t="s">
         <v>26</v>
@@ -5192,8 +5424,11 @@
         <f t="shared" si="3"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W77">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A78" s="4"/>
       <c r="B78" s="4" t="s">
         <v>27</v>
@@ -5255,8 +5490,11 @@
         <f t="shared" si="3"/>
         <v>328.08299999999997</v>
       </c>
-    </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W78">
+        <v>15.428571428571431</v>
+      </c>
+    </row>
+    <row r="79" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A79" s="4"/>
       <c r="B79" s="4" t="s">
         <v>27</v>
@@ -5312,8 +5550,11 @@
         <f t="shared" si="3"/>
         <v>328.08299999999997</v>
       </c>
-    </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W79">
+        <v>15.428571428571431</v>
+      </c>
+    </row>
+    <row r="80" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A80" s="4"/>
       <c r="B80" s="4" t="s">
         <v>27</v>
@@ -5369,8 +5610,11 @@
         <f t="shared" si="3"/>
         <v>328.08299999999997</v>
       </c>
-    </row>
-    <row r="81" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W80">
+        <v>15.428571428571431</v>
+      </c>
+    </row>
+    <row r="81" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A81" s="4"/>
       <c r="B81" s="4" t="s">
         <v>27</v>
@@ -5426,8 +5670,11 @@
         <f t="shared" si="3"/>
         <v>328.08299999999997</v>
       </c>
-    </row>
-    <row r="82" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W81">
+        <v>15.428571428571431</v>
+      </c>
+    </row>
+    <row r="82" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A82" s="4"/>
       <c r="B82" s="4" t="s">
         <v>27</v>
@@ -5483,8 +5730,11 @@
         <f t="shared" si="3"/>
         <v>328.08299999999997</v>
       </c>
-    </row>
-    <row r="83" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W82">
+        <v>15.428571428571431</v>
+      </c>
+    </row>
+    <row r="83" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A83" s="4"/>
       <c r="B83" s="4" t="s">
         <v>27</v>
@@ -5540,8 +5790,11 @@
         <f t="shared" si="3"/>
         <v>328.08299999999997</v>
       </c>
-    </row>
-    <row r="84" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W83">
+        <v>15.428571428571431</v>
+      </c>
+    </row>
+    <row r="84" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A84" s="4"/>
       <c r="B84" s="4" t="s">
         <v>27</v>
@@ -5597,8 +5850,11 @@
         <f t="shared" si="3"/>
         <v>328.08299999999997</v>
       </c>
-    </row>
-    <row r="85" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W84">
+        <v>15.428571428571431</v>
+      </c>
+    </row>
+    <row r="85" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A85" s="4"/>
       <c r="B85" s="4" t="s">
         <v>27</v>
@@ -5654,8 +5910,11 @@
         <f t="shared" si="3"/>
         <v>328.08299999999997</v>
       </c>
-    </row>
-    <row r="86" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W85">
+        <v>15.428571428571431</v>
+      </c>
+    </row>
+    <row r="86" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A86" s="4"/>
       <c r="B86" s="4" t="s">
         <v>27</v>
@@ -5713,8 +5972,11 @@
         <f t="shared" si="3"/>
         <v>328.08299999999997</v>
       </c>
-    </row>
-    <row r="87" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W86">
+        <v>15.428571428571431</v>
+      </c>
+    </row>
+    <row r="87" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A87" s="4"/>
       <c r="B87" s="4" t="s">
         <v>28</v>
@@ -5775,8 +6037,11 @@
         <f t="shared" si="3"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="88" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W87">
+        <v>14.399999999999999</v>
+      </c>
+    </row>
+    <row r="88" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A88" s="4"/>
       <c r="B88" s="4" t="s">
         <v>28</v>
@@ -5832,8 +6097,11 @@
         <f t="shared" si="3"/>
         <v>94.706625999999986</v>
       </c>
-    </row>
-    <row r="89" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W88">
+        <v>12.470399999999998</v>
+      </c>
+    </row>
+    <row r="89" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A89" s="4"/>
       <c r="B89" s="4" t="s">
         <v>28</v>
@@ -5893,8 +6161,11 @@
         <f t="shared" si="3"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="90" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W89">
+        <v>14.399999999999999</v>
+      </c>
+    </row>
+    <row r="90" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A90" s="4"/>
       <c r="B90" s="4" t="s">
         <v>29</v>
@@ -5950,8 +6221,11 @@
         <f t="shared" si="3"/>
         <v>82.020749999999992</v>
       </c>
-    </row>
-    <row r="91" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W90">
+        <v>10.799999999999999</v>
+      </c>
+    </row>
+    <row r="91" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A91" s="4"/>
       <c r="B91" s="4" t="s">
         <v>29</v>
@@ -6007,8 +6281,11 @@
         <f t="shared" si="3"/>
         <v>82.020749999999992</v>
       </c>
-    </row>
-    <row r="92" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W91">
+        <v>10.799999999999999</v>
+      </c>
+    </row>
+    <row r="92" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A92" s="4"/>
       <c r="B92" s="4" t="s">
         <v>29</v>
@@ -6064,8 +6341,11 @@
         <f t="shared" si="3"/>
         <v>82.020749999999992</v>
       </c>
-    </row>
-    <row r="93" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W92">
+        <v>10.799999999999999</v>
+      </c>
+    </row>
+    <row r="93" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A93" s="4"/>
       <c r="B93" s="4" t="s">
         <v>29</v>
@@ -6121,8 +6401,11 @@
         <f t="shared" si="3"/>
         <v>82.020749999999992</v>
       </c>
-    </row>
-    <row r="94" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W93">
+        <v>10.799999999999999</v>
+      </c>
+    </row>
+    <row r="94" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A94" s="4"/>
       <c r="B94" s="4" t="s">
         <v>29</v>
@@ -6178,8 +6461,11 @@
         <f t="shared" si="3"/>
         <v>82.020749999999992</v>
       </c>
-    </row>
-    <row r="95" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W94">
+        <v>10.799999999999999</v>
+      </c>
+    </row>
+    <row r="95" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A95" s="4"/>
       <c r="B95" s="4" t="s">
         <v>29</v>
@@ -6235,8 +6521,11 @@
         <f t="shared" si="3"/>
         <v>82.020749999999992</v>
       </c>
-    </row>
-    <row r="96" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W95">
+        <v>10.799999999999999</v>
+      </c>
+    </row>
+    <row r="96" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A96" s="4"/>
       <c r="B96" s="4" t="s">
         <v>29</v>
@@ -6292,8 +6581,11 @@
         <f t="shared" si="3"/>
         <v>82.020749999999992</v>
       </c>
-    </row>
-    <row r="97" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W96">
+        <v>10.799999999999999</v>
+      </c>
+    </row>
+    <row r="97" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A97" s="4"/>
       <c r="B97" s="4" t="s">
         <v>29</v>
@@ -6353,8 +6645,11 @@
         <f t="shared" si="3"/>
         <v>82.020749999999992</v>
       </c>
-    </row>
-    <row r="98" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W97">
+        <v>10.799999999999999</v>
+      </c>
+    </row>
+    <row r="98" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A98" s="4"/>
       <c r="B98" s="4" t="s">
         <v>29</v>
@@ -6410,8 +6705,11 @@
         <f t="shared" si="3"/>
         <v>82.020749999999992</v>
       </c>
-    </row>
-    <row r="99" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W98">
+        <v>10.799999999999999</v>
+      </c>
+    </row>
+    <row r="99" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A99" s="4"/>
       <c r="B99" s="4" t="s">
         <v>30</v>
@@ -6467,8 +6765,11 @@
         <f t="shared" si="3"/>
         <v>82.020749999999992</v>
       </c>
-    </row>
-    <row r="100" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W99">
+        <v>10.799999999999999</v>
+      </c>
+    </row>
+    <row r="100" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A100" s="4"/>
       <c r="B100" s="4" t="s">
         <v>30</v>
@@ -6524,8 +6825,11 @@
         <f t="shared" si="3"/>
         <v>82.020749999999992</v>
       </c>
-    </row>
-    <row r="101" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W100">
+        <v>10.799999999999999</v>
+      </c>
+    </row>
+    <row r="101" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A101" s="4"/>
       <c r="B101" s="4" t="s">
         <v>30</v>
@@ -6584,8 +6888,11 @@
         <f t="shared" si="3"/>
         <v>82.020749999999992</v>
       </c>
-    </row>
-    <row r="102" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W101">
+        <v>10.799999999999999</v>
+      </c>
+    </row>
+    <row r="102" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A102" s="4"/>
       <c r="B102" s="4" t="s">
         <v>31</v>
@@ -6646,8 +6953,11 @@
         <f t="shared" si="3"/>
         <v>38.276350000000001</v>
       </c>
-    </row>
-    <row r="103" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W102">
+        <v>4.8461538461538467</v>
+      </c>
+    </row>
+    <row r="103" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A103" s="4"/>
       <c r="B103" s="4" t="s">
         <v>32</v>
@@ -6703,8 +7013,11 @@
         <f t="shared" si="3"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="104" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W103">
+        <v>12.857142857142859</v>
+      </c>
+    </row>
+    <row r="104" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A104" s="4"/>
       <c r="B104" s="4" t="s">
         <v>32</v>
@@ -6760,8 +7073,11 @@
         <f t="shared" si="3"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="105" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W104">
+        <v>12.857142857142859</v>
+      </c>
+    </row>
+    <row r="105" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A105" s="4"/>
       <c r="B105" s="4" t="s">
         <v>32</v>
@@ -6817,8 +7133,11 @@
         <f t="shared" si="3"/>
         <v>87.488799999999998</v>
       </c>
-    </row>
-    <row r="106" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W105">
+        <v>10.285714285714286</v>
+      </c>
+    </row>
+    <row r="106" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A106" s="4"/>
       <c r="B106" s="4" t="s">
         <v>33</v>
@@ -6878,8 +7197,11 @@
         <f t="shared" si="3"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="107" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W106">
+        <v>12.857142857142859</v>
+      </c>
+    </row>
+    <row r="107" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A107" s="4"/>
       <c r="B107" s="4" t="s">
         <v>33</v>
@@ -6935,8 +7257,11 @@
         <f t="shared" si="3"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="108" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W107">
+        <v>12.857142857142859</v>
+      </c>
+    </row>
+    <row r="108" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A108" s="4"/>
       <c r="B108" s="4" t="s">
         <v>33</v>
@@ -6992,8 +7317,11 @@
         <f t="shared" si="3"/>
         <v>98.424899999999994</v>
       </c>
-    </row>
-    <row r="109" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W108">
+        <v>11.571428571428573</v>
+      </c>
+    </row>
+    <row r="109" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A109" s="4"/>
       <c r="B109" s="4" t="s">
         <v>33</v>
@@ -7049,8 +7377,11 @@
         <f t="shared" si="3"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="110" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W109">
+        <v>12.857142857142859</v>
+      </c>
+    </row>
+    <row r="110" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A110" s="4"/>
       <c r="B110" s="4" t="s">
         <v>33</v>
@@ -7106,8 +7437,11 @@
         <f t="shared" si="3"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="111" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W110">
+        <v>12.857142857142859</v>
+      </c>
+    </row>
+    <row r="111" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A111" s="4"/>
       <c r="B111" s="4" t="s">
         <v>34</v>
@@ -7163,8 +7497,11 @@
         <f t="shared" si="3"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="112" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W111">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="112" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A112" s="4"/>
       <c r="B112" s="4" t="s">
         <v>34</v>
@@ -7220,8 +7557,11 @@
         <f t="shared" si="3"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="113" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W112">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="113" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A113" s="4"/>
       <c r="B113" s="4" t="s">
         <v>34</v>
@@ -7277,8 +7617,11 @@
         <f t="shared" si="3"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="114" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W113">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="114" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A114" s="4"/>
       <c r="B114" s="4" t="s">
         <v>34</v>
@@ -7334,8 +7677,11 @@
         <f t="shared" si="3"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="115" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W114">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="115" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A115" s="4"/>
       <c r="B115" s="4" t="s">
         <v>34</v>
@@ -7395,8 +7741,11 @@
         <f t="shared" si="3"/>
         <v>177.16481999999999</v>
       </c>
-    </row>
-    <row r="116" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W115">
+        <v>19.439999999999998</v>
+      </c>
+    </row>
+    <row r="116" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A116" s="4"/>
       <c r="B116" s="4" t="s">
         <v>34</v>
@@ -7452,8 +7801,11 @@
         <f t="shared" si="3"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="117" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W116">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="117" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A117" s="4"/>
       <c r="B117" s="4" t="s">
         <v>34</v>
@@ -7509,8 +7861,11 @@
         <f t="shared" si="3"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="118" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W117">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="118" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A118" s="4"/>
       <c r="B118" s="4" t="s">
         <v>35</v>
@@ -7566,8 +7921,11 @@
         <f t="shared" si="3"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="119" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W118">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="119" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A119" s="4"/>
       <c r="B119" s="4" t="s">
         <v>35</v>
@@ -7623,8 +7981,11 @@
         <f t="shared" si="3"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="120" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W119">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="120" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A120" s="4"/>
       <c r="B120" s="4" t="s">
         <v>35</v>
@@ -7680,8 +8041,11 @@
         <f t="shared" si="3"/>
         <v>43.744399999999999</v>
       </c>
-    </row>
-    <row r="121" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W120">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="121" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A121" s="4"/>
       <c r="B121" s="4" t="s">
         <v>35</v>
@@ -7737,8 +8101,11 @@
         <f t="shared" si="3"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="122" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W121">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="122" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A122" s="4"/>
       <c r="B122" s="4" t="s">
         <v>35</v>
@@ -7794,8 +8161,11 @@
         <f t="shared" si="3"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="123" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W122">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="123" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A123" s="4"/>
       <c r="B123" s="4" t="s">
         <v>36</v>
@@ -7851,8 +8221,11 @@
         <f t="shared" si="3"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="124" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W123">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="124" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A124" s="4"/>
       <c r="B124" s="4" t="s">
         <v>36</v>
@@ -7912,8 +8285,11 @@
         <f t="shared" si="3"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="125" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W124">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="125" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A125" s="4"/>
       <c r="B125" s="4" t="s">
         <v>36</v>
@@ -7969,8 +8345,11 @@
         <f t="shared" si="3"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="126" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W125">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="126" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A126" s="4"/>
       <c r="B126" s="4" t="s">
         <v>36</v>
@@ -8026,8 +8405,11 @@
         <f t="shared" si="3"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="127" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W126">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="127" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A127" s="4"/>
       <c r="B127" s="4" t="s">
         <v>36</v>
@@ -8083,8 +8465,11 @@
         <f t="shared" si="3"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="128" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W127">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="128" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A128" s="4"/>
       <c r="B128" s="4" t="s">
         <v>36</v>
@@ -8140,8 +8525,11 @@
         <f t="shared" si="3"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="129" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W128">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="129" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A129" s="4"/>
       <c r="B129" s="4" t="s">
         <v>36</v>
@@ -8197,8 +8585,11 @@
         <f t="shared" si="3"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="130" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W129">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="130" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A130" s="4"/>
       <c r="B130" s="4" t="s">
         <v>36</v>
@@ -8254,8 +8645,11 @@
         <f t="shared" si="3"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="131" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W130">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="131" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A131" s="4"/>
       <c r="B131" s="4" t="s">
         <v>36</v>
@@ -8311,8 +8705,11 @@
         <f t="shared" ref="V131:V153" si="5">D131 * 1.09361</f>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="132" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W131">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="132" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A132" s="4"/>
       <c r="B132" s="4" t="s">
         <v>36</v>
@@ -8368,8 +8765,11 @@
         <f t="shared" si="5"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="133" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W132">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="133" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A133" s="4"/>
       <c r="B133" s="4" t="s">
         <v>36</v>
@@ -8429,8 +8829,11 @@
         <f t="shared" si="5"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="134" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W133">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="134" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A134" s="4"/>
       <c r="B134" s="4" t="s">
         <v>36</v>
@@ -8486,8 +8889,11 @@
         <f t="shared" si="5"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="135" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W134">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="135" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A135" s="4"/>
       <c r="B135" s="4" t="s">
         <v>36</v>
@@ -8543,8 +8949,11 @@
         <f t="shared" si="5"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="136" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W135">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="136" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A136" s="4"/>
       <c r="B136" s="4" t="s">
         <v>36</v>
@@ -8600,8 +9009,11 @@
         <f t="shared" si="5"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="137" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W136">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="137" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A137" s="4"/>
       <c r="B137" s="4" t="s">
         <v>36</v>
@@ -8657,8 +9069,11 @@
         <f t="shared" si="5"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="138" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W137">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="138" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A138" s="4"/>
       <c r="B138" s="4" t="s">
         <v>36</v>
@@ -8714,8 +9129,11 @@
         <f t="shared" si="5"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="139" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W138">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="139" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A139" s="4"/>
       <c r="B139" s="4" t="s">
         <v>36</v>
@@ -8771,8 +9189,11 @@
         <f t="shared" si="5"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="140" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W139">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="140" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A140" s="4"/>
       <c r="B140" s="4" t="s">
         <v>36</v>
@@ -8828,8 +9249,11 @@
         <f t="shared" si="5"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="141" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W140">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="141" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A141" s="4"/>
       <c r="B141" s="4" t="s">
         <v>36</v>
@@ -8885,8 +9309,11 @@
         <f t="shared" si="5"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="142" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W141">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="142" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A142" s="4"/>
       <c r="B142" s="4" t="s">
         <v>36</v>
@@ -8946,8 +9373,11 @@
         <f t="shared" si="5"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="143" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W142">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="143" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A143" s="4"/>
       <c r="B143" s="4" t="s">
         <v>36</v>
@@ -9003,8 +9433,11 @@
         <f t="shared" si="5"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="144" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W143">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="144" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A144" s="4"/>
       <c r="B144" s="4" t="s">
         <v>36</v>
@@ -9060,8 +9493,11 @@
         <f t="shared" si="5"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="145" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W144">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="145" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A145" s="4"/>
       <c r="B145" s="4" t="s">
         <v>37</v>
@@ -9117,8 +9553,11 @@
         <f t="shared" si="5"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="146" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W145">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="146" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A146" s="4"/>
       <c r="B146" s="4" t="s">
         <v>37</v>
@@ -9174,8 +9613,11 @@
         <f t="shared" si="5"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="147" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W146">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="147" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A147" s="4"/>
       <c r="B147" s="4" t="s">
         <v>37</v>
@@ -9231,8 +9673,11 @@
         <f t="shared" si="5"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="148" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W147">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="148" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A148" s="4"/>
       <c r="B148" s="4" t="s">
         <v>38</v>
@@ -9288,8 +9733,11 @@
         <f t="shared" si="5"/>
         <v>54.680499999999995</v>
       </c>
-    </row>
-    <row r="149" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W148">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="149" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A149" s="4"/>
       <c r="B149" s="4" t="s">
         <v>38</v>
@@ -9345,8 +9793,11 @@
         <f t="shared" si="5"/>
         <v>201.22424000000001</v>
       </c>
-    </row>
-    <row r="150" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W149">
+        <v>33.119999999999997</v>
+      </c>
+    </row>
+    <row r="150" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A150" s="4"/>
       <c r="B150" s="4" t="s">
         <v>38</v>
@@ -9402,8 +9853,11 @@
         <f t="shared" si="5"/>
         <v>43.744399999999999</v>
       </c>
-    </row>
-    <row r="151" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W150">
+        <v>7.1999999999999993</v>
+      </c>
+    </row>
+    <row r="151" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A151" s="4"/>
       <c r="B151" s="4" t="s">
         <v>39</v>
@@ -9462,8 +9916,11 @@
         <f t="shared" si="5"/>
         <v>38.276350000000001</v>
       </c>
-    </row>
-    <row r="152" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W151">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B152" s="4" t="s">
         <v>79</v>
       </c>
@@ -9517,8 +9974,12 @@
         <f t="shared" si="5"/>
         <v>109.36099999999999</v>
       </c>
-    </row>
-    <row r="153" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W152">
+        <f xml:space="preserve"> V152/(U152*0.488889)</f>
+        <v>23.999929586474448</v>
+      </c>
+    </row>
+    <row r="153" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B153" s="4" t="s">
         <v>79</v>
       </c>
@@ -9571,6 +10032,10 @@
       <c r="V153">
         <f t="shared" si="5"/>
         <v>109.36099999999999</v>
+      </c>
+      <c r="W153">
+        <f xml:space="preserve"> V153/(U153*0.488889)</f>
+        <v>23.999929586474448</v>
       </c>
     </row>
   </sheetData>

</xml_diff>